<commit_message>
vlsm edited and pkt dumb shit
</commit_message>
<xml_diff>
--- a/Documentations/VLANs/VLSM-tablazat.xlsx
+++ b/Documentations/VLANs/VLSM-tablazat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\aromas-cubanos\Documentations\VLANs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D8953E-BE70-487A-B6D6-DEC2EA353C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5078C028-35F0-4097-B5E8-236C18C7B407}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{012D1D82-EB97-4B95-AC21-450975C8649A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{012D1D82-EB97-4B95-AC21-450975C8649A}"/>
   </bookViews>
   <sheets>
     <sheet name="plain" sheetId="1" r:id="rId1"/>
@@ -1044,6 +1044,12 @@
     <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1150,12 +1156,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -5154,61 +5154,52 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="H130:H257"/>
-    <mergeCell ref="F162:F193"/>
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="G130:G193"/>
-    <mergeCell ref="G194:G257"/>
-    <mergeCell ref="E178:E193"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="E226:E241"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="E146:E161"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="D194:D201"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="D146:D153"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="D170:D177"/>
-    <mergeCell ref="D178:D185"/>
-    <mergeCell ref="D186:D193"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="D138:D145"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="C190:C193"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="C166:C169"/>
     <mergeCell ref="C242:C245"/>
     <mergeCell ref="C246:C249"/>
     <mergeCell ref="C250:C253"/>
@@ -5233,52 +5224,61 @@
     <mergeCell ref="C170:C173"/>
     <mergeCell ref="C174:C177"/>
     <mergeCell ref="D98:D105"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="C190:C193"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="C134:C137"/>
-    <mergeCell ref="C138:C141"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="D138:D145"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="D90:D97"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="D194:D201"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="D146:D153"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="D170:D177"/>
+    <mergeCell ref="D178:D185"/>
+    <mergeCell ref="D186:D193"/>
+    <mergeCell ref="E178:E193"/>
+    <mergeCell ref="E194:E209"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="E146:E161"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="H130:H257"/>
+    <mergeCell ref="F162:F193"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="G130:G193"/>
+    <mergeCell ref="G194:G257"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -5289,8 +5289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709A4C10-0955-4D97-86D1-D5085866A222}">
   <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE65" sqref="AE65"/>
+    <sheetView tabSelected="1" topLeftCell="N4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5344,7 +5344,7 @@
       <c r="G1" s="3">
         <v>0</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="98" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -5356,7 +5356,7 @@
       <c r="L1" s="3">
         <v>0</v>
       </c>
-      <c r="M1" s="102" t="s">
+      <c r="M1" s="104" t="s">
         <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -5368,7 +5368,7 @@
       <c r="Q1" s="42">
         <v>0</v>
       </c>
-      <c r="R1" s="108" t="s">
+      <c r="R1" s="110" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -5390,7 +5390,7 @@
       <c r="G2" s="6">
         <v>1</v>
       </c>
-      <c r="H2" s="97"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="7"/>
       <c r="K2" s="12" t="s">
         <v>76</v>
@@ -5398,7 +5398,7 @@
       <c r="L2" s="6">
         <v>1</v>
       </c>
-      <c r="M2" s="103"/>
+      <c r="M2" s="105"/>
       <c r="N2" s="7"/>
       <c r="P2" s="12" t="s">
         <v>83</v>
@@ -5406,16 +5406,16 @@
       <c r="Q2" s="41">
         <v>1</v>
       </c>
-      <c r="R2" s="109"/>
+      <c r="R2" s="111"/>
       <c r="S2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="90" t="s">
+      <c r="AA2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="92"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="94"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -5432,7 +5432,7 @@
       <c r="G3" s="6">
         <v>2</v>
       </c>
-      <c r="H3" s="97"/>
+      <c r="H3" s="99"/>
       <c r="I3" s="7"/>
       <c r="K3" s="12" t="s">
         <v>76</v>
@@ -5440,7 +5440,7 @@
       <c r="L3" s="6">
         <v>2</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="7"/>
       <c r="P3" s="12" t="s">
         <v>83</v>
@@ -5448,7 +5448,7 @@
       <c r="Q3" s="41">
         <v>2</v>
       </c>
-      <c r="R3" s="109"/>
+      <c r="R3" s="111"/>
       <c r="S3" s="7" t="s">
         <v>35</v>
       </c>
@@ -5480,7 +5480,7 @@
       <c r="G4" s="6">
         <v>3</v>
       </c>
-      <c r="H4" s="97"/>
+      <c r="H4" s="99"/>
       <c r="I4" s="7"/>
       <c r="K4" s="12" t="s">
         <v>76</v>
@@ -5488,7 +5488,7 @@
       <c r="L4" s="6">
         <v>3</v>
       </c>
-      <c r="M4" s="103"/>
+      <c r="M4" s="105"/>
       <c r="N4" s="7"/>
       <c r="P4" s="12" t="s">
         <v>83</v>
@@ -5496,7 +5496,7 @@
       <c r="Q4" s="41">
         <v>3</v>
       </c>
-      <c r="R4" s="109"/>
+      <c r="R4" s="111"/>
       <c r="S4" s="7"/>
       <c r="AA4" s="23">
         <v>10</v>
@@ -5526,7 +5526,7 @@
       <c r="G5" s="6">
         <v>4</v>
       </c>
-      <c r="H5" s="97"/>
+      <c r="H5" s="99"/>
       <c r="I5" s="7"/>
       <c r="K5" s="12" t="s">
         <v>76</v>
@@ -5534,7 +5534,7 @@
       <c r="L5" s="6">
         <v>4</v>
       </c>
-      <c r="M5" s="103"/>
+      <c r="M5" s="105"/>
       <c r="N5" s="7"/>
       <c r="P5" s="12" t="s">
         <v>83</v>
@@ -5542,7 +5542,7 @@
       <c r="Q5" s="41">
         <v>4</v>
       </c>
-      <c r="R5" s="109"/>
+      <c r="R5" s="111"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -5560,7 +5560,7 @@
       <c r="G6" s="6">
         <v>5</v>
       </c>
-      <c r="H6" s="97"/>
+      <c r="H6" s="99"/>
       <c r="I6" s="7"/>
       <c r="K6" s="32" t="s">
         <v>76</v>
@@ -5568,7 +5568,7 @@
       <c r="L6" s="33">
         <v>254</v>
       </c>
-      <c r="M6" s="103"/>
+      <c r="M6" s="105"/>
       <c r="N6" s="34" t="s">
         <v>44</v>
       </c>
@@ -5578,14 +5578,14 @@
       <c r="Q6" s="71">
         <v>254</v>
       </c>
-      <c r="R6" s="109"/>
+      <c r="R6" s="111"/>
       <c r="S6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="AA6" s="94" t="s">
+      <c r="AA6" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="95"/>
+      <c r="AB6" s="97"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -5602,7 +5602,7 @@
       <c r="G7" s="6">
         <v>6</v>
       </c>
-      <c r="H7" s="97"/>
+      <c r="H7" s="99"/>
       <c r="I7" s="7"/>
       <c r="K7" s="11" t="s">
         <v>76</v>
@@ -5610,7 +5610,7 @@
       <c r="L7" s="3">
         <v>255</v>
       </c>
-      <c r="M7" s="103"/>
+      <c r="M7" s="105"/>
       <c r="N7" s="4" t="s">
         <v>19</v>
       </c>
@@ -5620,7 +5620,7 @@
       <c r="Q7" s="42">
         <v>255</v>
       </c>
-      <c r="R7" s="110"/>
+      <c r="R7" s="112"/>
       <c r="S7" s="4" t="s">
         <v>19</v>
       </c>
@@ -5646,7 +5646,7 @@
       <c r="G8" s="6">
         <v>7</v>
       </c>
-      <c r="H8" s="97"/>
+      <c r="H8" s="99"/>
       <c r="I8" s="7"/>
       <c r="K8" s="11" t="s">
         <v>77</v>
@@ -5654,7 +5654,7 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="103"/>
+      <c r="M8" s="105"/>
       <c r="N8" s="4" t="s">
         <v>23</v>
       </c>
@@ -5680,7 +5680,7 @@
       <c r="G9" s="6">
         <v>8</v>
       </c>
-      <c r="H9" s="97"/>
+      <c r="H9" s="99"/>
       <c r="I9" s="7"/>
       <c r="K9" s="12" t="s">
         <v>77</v>
@@ -5688,7 +5688,7 @@
       <c r="L9" s="6">
         <v>1</v>
       </c>
-      <c r="M9" s="103"/>
+      <c r="M9" s="105"/>
       <c r="N9" s="7"/>
       <c r="P9" s="64" t="s">
         <v>107</v>
@@ -5696,7 +5696,7 @@
       <c r="Q9" s="42">
         <v>0</v>
       </c>
-      <c r="R9" s="104" t="s">
+      <c r="R9" s="106" t="s">
         <v>20</v>
       </c>
       <c r="S9" s="4" t="s">
@@ -5724,7 +5724,7 @@
       <c r="G10" s="6">
         <v>9</v>
       </c>
-      <c r="H10" s="97"/>
+      <c r="H10" s="99"/>
       <c r="I10" s="7"/>
       <c r="K10" s="12" t="s">
         <v>77</v>
@@ -5732,7 +5732,7 @@
       <c r="L10" s="6">
         <v>2</v>
       </c>
-      <c r="M10" s="103"/>
+      <c r="M10" s="105"/>
       <c r="N10" s="7"/>
       <c r="P10" s="65" t="s">
         <v>107</v>
@@ -5740,7 +5740,7 @@
       <c r="Q10" s="41">
         <v>1</v>
       </c>
-      <c r="R10" s="104"/>
+      <c r="R10" s="106"/>
       <c r="S10" s="7" t="s">
         <v>21</v>
       </c>
@@ -5766,7 +5766,7 @@
       <c r="G11" s="6">
         <v>10</v>
       </c>
-      <c r="H11" s="97"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="7"/>
       <c r="K11" s="12" t="s">
         <v>77</v>
@@ -5774,7 +5774,7 @@
       <c r="L11" s="6">
         <v>3</v>
       </c>
-      <c r="M11" s="103"/>
+      <c r="M11" s="105"/>
       <c r="N11" s="7"/>
       <c r="P11" s="65" t="s">
         <v>107</v>
@@ -5782,7 +5782,7 @@
       <c r="Q11" s="41">
         <v>2</v>
       </c>
-      <c r="R11" s="104"/>
+      <c r="R11" s="106"/>
       <c r="S11" s="7" t="s">
         <v>22</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="G12" s="6">
         <v>11</v>
       </c>
-      <c r="H12" s="97"/>
+      <c r="H12" s="99"/>
       <c r="I12" s="7"/>
       <c r="K12" s="12" t="s">
         <v>77</v>
@@ -5810,7 +5810,7 @@
       <c r="L12" s="6">
         <v>4</v>
       </c>
-      <c r="M12" s="103"/>
+      <c r="M12" s="105"/>
       <c r="N12" s="7"/>
       <c r="P12" s="84" t="s">
         <v>107</v>
@@ -5818,7 +5818,7 @@
       <c r="Q12" s="43">
         <v>254</v>
       </c>
-      <c r="R12" s="104"/>
+      <c r="R12" s="106"/>
       <c r="S12" s="37" t="s">
         <v>44</v>
       </c>
@@ -5842,7 +5842,7 @@
       <c r="G13" s="6">
         <v>12</v>
       </c>
-      <c r="H13" s="97"/>
+      <c r="H13" s="99"/>
       <c r="I13" s="7"/>
       <c r="K13" s="32" t="s">
         <v>77</v>
@@ -5850,7 +5850,7 @@
       <c r="L13" s="33">
         <v>254</v>
       </c>
-      <c r="M13" s="103"/>
+      <c r="M13" s="105"/>
       <c r="N13" s="34" t="s">
         <v>44</v>
       </c>
@@ -5860,7 +5860,7 @@
       <c r="Q13" s="42">
         <v>255</v>
       </c>
-      <c r="R13" s="104"/>
+      <c r="R13" s="106"/>
       <c r="S13" s="4" t="s">
         <v>19</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="G14" s="6">
         <v>13</v>
       </c>
-      <c r="H14" s="97"/>
+      <c r="H14" s="99"/>
       <c r="I14" s="7"/>
       <c r="K14" s="11" t="s">
         <v>77</v>
@@ -5892,7 +5892,7 @@
       <c r="L14" s="3">
         <v>255</v>
       </c>
-      <c r="M14" s="103"/>
+      <c r="M14" s="105"/>
       <c r="N14" s="4" t="s">
         <v>19</v>
       </c>
@@ -5916,7 +5916,7 @@
       <c r="G15" s="6">
         <v>14</v>
       </c>
-      <c r="H15" s="97"/>
+      <c r="H15" s="99"/>
       <c r="I15" s="7"/>
       <c r="K15" s="11" t="s">
         <v>78</v>
@@ -5924,7 +5924,7 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="103"/>
+      <c r="M15" s="105"/>
       <c r="N15" s="4" t="s">
         <v>23</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>115</v>
       </c>
       <c r="T15" s="73" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="47"/>
       <c r="AB15" s="47"/>
@@ -5963,7 +5963,7 @@
       <c r="G16" s="6">
         <v>15</v>
       </c>
-      <c r="H16" s="97"/>
+      <c r="H16" s="99"/>
       <c r="I16" s="7"/>
       <c r="K16" s="12" t="s">
         <v>78</v>
@@ -5971,7 +5971,7 @@
       <c r="L16" s="6">
         <v>1</v>
       </c>
-      <c r="M16" s="103"/>
+      <c r="M16" s="105"/>
       <c r="N16" s="7"/>
       <c r="P16" s="77" t="s">
         <v>64</v>
@@ -5980,10 +5980,10 @@
         <v>1</v>
       </c>
       <c r="R16" s="89"/>
-      <c r="S16" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="T16" s="80"/>
+      <c r="S16" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" s="74"/>
       <c r="AA16" s="47"/>
       <c r="AB16" s="47"/>
       <c r="AC16" s="47"/>
@@ -6003,7 +6003,7 @@
       <c r="G17" s="6">
         <v>16</v>
       </c>
-      <c r="H17" s="97"/>
+      <c r="H17" s="99"/>
       <c r="I17" s="7"/>
       <c r="K17" s="12" t="s">
         <v>78</v>
@@ -6011,7 +6011,7 @@
       <c r="L17" s="6">
         <v>2</v>
       </c>
-      <c r="M17" s="103"/>
+      <c r="M17" s="105"/>
       <c r="N17" s="7"/>
       <c r="P17" s="77" t="s">
         <v>64</v>
@@ -6020,10 +6020,10 @@
         <v>2</v>
       </c>
       <c r="R17" s="89"/>
-      <c r="S17" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="T17" s="80"/>
+      <c r="S17" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" s="74"/>
       <c r="AA17" s="45"/>
       <c r="AB17" s="46"/>
       <c r="AC17" s="46"/>
@@ -6043,7 +6043,7 @@
       <c r="G18" s="6">
         <v>17</v>
       </c>
-      <c r="H18" s="97"/>
+      <c r="H18" s="99"/>
       <c r="I18" s="7"/>
       <c r="K18" s="12" t="s">
         <v>78</v>
@@ -6051,17 +6051,17 @@
       <c r="L18" s="6">
         <v>3</v>
       </c>
-      <c r="M18" s="103"/>
+      <c r="M18" s="105"/>
       <c r="N18" s="7"/>
-      <c r="P18" s="70" t="s">
+      <c r="P18" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="Q18" s="70">
-        <v>7</v>
+      <c r="Q18" s="77">
+        <v>3</v>
       </c>
       <c r="R18" s="89"/>
-      <c r="S18" s="69" t="s">
-        <v>19</v>
+      <c r="S18" s="41" t="s">
+        <v>60</v>
       </c>
       <c r="T18" s="74"/>
       <c r="AA18" s="29"/>
@@ -6084,7 +6084,7 @@
       <c r="G19" s="6">
         <v>18</v>
       </c>
-      <c r="H19" s="97"/>
+      <c r="H19" s="99"/>
       <c r="I19" s="7"/>
       <c r="K19" s="12" t="s">
         <v>78</v>
@@ -6092,21 +6092,17 @@
       <c r="L19" s="6">
         <v>4</v>
       </c>
-      <c r="M19" s="103"/>
+      <c r="M19" s="105"/>
       <c r="N19" s="7"/>
-      <c r="P19" s="70" t="s">
+      <c r="P19" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="Q19" s="70">
-        <v>8</v>
+      <c r="Q19" s="77">
+        <v>4</v>
       </c>
       <c r="R19" s="89"/>
-      <c r="S19" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="T19" s="73" t="s">
-        <v>0</v>
-      </c>
+      <c r="S19" s="41"/>
+      <c r="T19" s="74"/>
       <c r="AA19" s="29"/>
       <c r="AB19" s="29"/>
       <c r="AC19" s="29"/>
@@ -6127,7 +6123,7 @@
       <c r="G20" s="6">
         <v>19</v>
       </c>
-      <c r="H20" s="97"/>
+      <c r="H20" s="99"/>
       <c r="I20" s="7"/>
       <c r="K20" s="32" t="s">
         <v>78</v>
@@ -6135,7 +6131,7 @@
       <c r="L20" s="33">
         <v>254</v>
       </c>
-      <c r="M20" s="103"/>
+      <c r="M20" s="105"/>
       <c r="N20" s="34" t="s">
         <v>44</v>
       </c>
@@ -6143,12 +6139,10 @@
         <v>64</v>
       </c>
       <c r="Q20" s="41">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R20" s="89"/>
-      <c r="S20" s="41" t="s">
-        <v>52</v>
-      </c>
+      <c r="S20" s="41"/>
       <c r="T20" s="74"/>
       <c r="AA20" s="29"/>
       <c r="AB20" s="29"/>
@@ -6170,7 +6164,7 @@
       <c r="G21" s="6">
         <v>20</v>
       </c>
-      <c r="H21" s="97"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="7"/>
       <c r="K21" s="11" t="s">
         <v>78</v>
@@ -6178,7 +6172,7 @@
       <c r="L21" s="3">
         <v>255</v>
       </c>
-      <c r="M21" s="103"/>
+      <c r="M21" s="105"/>
       <c r="N21" s="4" t="s">
         <v>19</v>
       </c>
@@ -6186,12 +6180,9 @@
         <v>64</v>
       </c>
       <c r="Q21" s="41">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R21" s="89"/>
-      <c r="S21" s="76" t="s">
-        <v>118</v>
-      </c>
       <c r="T21" s="74"/>
       <c r="AA21" s="29"/>
       <c r="AB21" s="29"/>
@@ -6213,19 +6204,19 @@
       <c r="G22" s="6">
         <v>21</v>
       </c>
-      <c r="H22" s="97"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="7"/>
       <c r="P22" s="70" t="s">
         <v>64</v>
       </c>
       <c r="Q22" s="70">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R22" s="89"/>
       <c r="S22" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="T22" s="74"/>
+      <c r="T22" s="75"/>
       <c r="AA22" s="29"/>
       <c r="AB22" s="29"/>
       <c r="AC22" s="29"/>
@@ -6246,7 +6237,7 @@
       <c r="G23" s="6">
         <v>22</v>
       </c>
-      <c r="H23" s="97"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="7"/>
       <c r="K23" s="11" t="s">
         <v>79</v>
@@ -6254,7 +6245,7 @@
       <c r="L23" s="3">
         <v>0</v>
       </c>
-      <c r="M23" s="93" t="s">
+      <c r="M23" s="95" t="s">
         <v>16</v>
       </c>
       <c r="N23" s="4" t="s">
@@ -6264,17 +6255,15 @@
         <v>64</v>
       </c>
       <c r="Q23" s="70">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="R23" s="89"/>
       <c r="S23" s="69" t="s">
         <v>115</v>
       </c>
       <c r="T23" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="29"/>
-      <c r="AB23" s="29"/>
+        <v>0</v>
+      </c>
       <c r="AC23" s="29"/>
       <c r="AD23" s="29"/>
     </row>
@@ -6293,7 +6282,7 @@
       <c r="G24" s="6">
         <v>23</v>
       </c>
-      <c r="H24" s="97"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="7"/>
       <c r="K24" s="12" t="s">
         <v>79</v>
@@ -6301,21 +6290,19 @@
       <c r="L24" s="6">
         <v>1</v>
       </c>
-      <c r="M24" s="93"/>
+      <c r="M24" s="95"/>
       <c r="N24" s="7"/>
       <c r="P24" s="41" t="s">
         <v>64</v>
       </c>
       <c r="Q24" s="41">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="R24" s="89"/>
-      <c r="S24" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="T24" s="74"/>
-      <c r="AA24" s="29"/>
-      <c r="AB24" s="29"/>
+      <c r="S24" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="T24" s="80"/>
       <c r="AC24" s="29"/>
       <c r="AD24" s="29"/>
     </row>
@@ -6334,7 +6321,7 @@
       <c r="G25" s="6">
         <v>24</v>
       </c>
-      <c r="H25" s="97"/>
+      <c r="H25" s="99"/>
       <c r="I25" s="7"/>
       <c r="K25" s="12" t="s">
         <v>79</v>
@@ -6342,19 +6329,19 @@
       <c r="L25" s="6">
         <v>2</v>
       </c>
-      <c r="M25" s="93"/>
+      <c r="M25" s="95"/>
       <c r="N25" s="7"/>
       <c r="P25" s="41" t="s">
         <v>64</v>
       </c>
       <c r="Q25" s="41">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R25" s="89"/>
-      <c r="S25" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="T25" s="74"/>
+      <c r="S25" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="T25" s="80"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -6371,7 +6358,7 @@
       <c r="G26" s="6">
         <v>25</v>
       </c>
-      <c r="H26" s="97"/>
+      <c r="H26" s="99"/>
       <c r="I26" s="7"/>
       <c r="K26" s="12" t="s">
         <v>79</v>
@@ -6379,17 +6366,17 @@
       <c r="L26" s="6">
         <v>3</v>
       </c>
-      <c r="M26" s="93"/>
+      <c r="M26" s="95"/>
       <c r="N26" s="7"/>
-      <c r="P26" s="41" t="s">
+      <c r="P26" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="Q26" s="41">
-        <v>15</v>
+      <c r="Q26" s="70">
+        <v>11</v>
       </c>
       <c r="R26" s="89"/>
-      <c r="S26" s="41" t="s">
-        <v>60</v>
+      <c r="S26" s="69" t="s">
+        <v>19</v>
       </c>
       <c r="T26" s="74"/>
     </row>
@@ -6408,7 +6395,7 @@
       <c r="G27" s="6">
         <v>26</v>
       </c>
-      <c r="H27" s="97"/>
+      <c r="H27" s="99"/>
       <c r="I27" s="7"/>
       <c r="K27" s="12" t="s">
         <v>79</v>
@@ -6416,17 +6403,21 @@
       <c r="L27" s="6">
         <v>4</v>
       </c>
-      <c r="M27" s="93"/>
+      <c r="M27" s="95"/>
       <c r="N27" s="7"/>
-      <c r="P27" s="41" t="s">
+      <c r="P27" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="41">
-        <v>16</v>
+      <c r="Q27" s="70">
+        <v>12</v>
       </c>
       <c r="R27" s="89"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="74"/>
+      <c r="S27" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="T27" s="73" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -6443,7 +6434,7 @@
       <c r="G28" s="6">
         <v>27</v>
       </c>
-      <c r="H28" s="97"/>
+      <c r="H28" s="99"/>
       <c r="I28" s="7"/>
       <c r="K28" s="12" t="s">
         <v>79</v>
@@ -6451,16 +6442,18 @@
       <c r="L28" s="6">
         <v>5</v>
       </c>
-      <c r="M28" s="93"/>
+      <c r="M28" s="95"/>
       <c r="N28" s="7"/>
       <c r="P28" s="41" t="s">
         <v>64</v>
       </c>
       <c r="Q28" s="41">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="R28" s="89"/>
-      <c r="S28" s="41"/>
+      <c r="S28" s="41" t="s">
+        <v>52</v>
+      </c>
       <c r="T28" s="74"/>
     </row>
     <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6478,7 +6471,7 @@
       <c r="G29" s="6">
         <v>28</v>
       </c>
-      <c r="H29" s="97"/>
+      <c r="H29" s="99"/>
       <c r="I29" s="7"/>
       <c r="K29" s="35" t="s">
         <v>79</v>
@@ -6486,7 +6479,7 @@
       <c r="L29" s="36">
         <v>254</v>
       </c>
-      <c r="M29" s="93"/>
+      <c r="M29" s="95"/>
       <c r="N29" s="37" t="s">
         <v>44</v>
       </c>
@@ -6494,9 +6487,12 @@
         <v>64</v>
       </c>
       <c r="Q29" s="68">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="R29" s="89"/>
+      <c r="S29" s="76" t="s">
+        <v>118</v>
+      </c>
       <c r="T29" s="74"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
@@ -6514,7 +6510,7 @@
       <c r="G30" s="6">
         <v>29</v>
       </c>
-      <c r="H30" s="97"/>
+      <c r="H30" s="99"/>
       <c r="I30" s="7"/>
       <c r="K30" s="11" t="s">
         <v>79</v>
@@ -6522,7 +6518,7 @@
       <c r="L30" s="3">
         <v>255</v>
       </c>
-      <c r="M30" s="93"/>
+      <c r="M30" s="95"/>
       <c r="N30" s="4" t="s">
         <v>19</v>
       </c>
@@ -6530,7 +6526,7 @@
         <v>64</v>
       </c>
       <c r="Q30" s="70">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R30" s="89"/>
       <c r="S30" s="69" t="s">
@@ -6553,7 +6549,7 @@
       <c r="G31" s="6">
         <v>30</v>
       </c>
-      <c r="H31" s="97"/>
+      <c r="H31" s="99"/>
       <c r="I31" s="7"/>
       <c r="P31" s="42" t="s">
         <v>65</v>
@@ -6581,7 +6577,7 @@
       <c r="G32" s="33">
         <v>254</v>
       </c>
-      <c r="H32" s="97"/>
+      <c r="H32" s="99"/>
       <c r="I32" s="34" t="s">
         <v>94</v>
       </c>
@@ -6591,7 +6587,7 @@
       <c r="L32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="105" t="s">
+      <c r="M32" s="107" t="s">
         <v>24</v>
       </c>
       <c r="N32" s="4" t="s">
@@ -6627,7 +6623,7 @@
       <c r="G33" s="3">
         <v>255</v>
       </c>
-      <c r="H33" s="98"/>
+      <c r="H33" s="100"/>
       <c r="I33" s="4" t="s">
         <v>19</v>
       </c>
@@ -6637,7 +6633,7 @@
       <c r="L33" s="6">
         <v>1</v>
       </c>
-      <c r="M33" s="106"/>
+      <c r="M33" s="108"/>
       <c r="N33" s="7"/>
       <c r="P33" s="41" t="s">
         <v>65</v>
@@ -6668,7 +6664,7 @@
       <c r="L34" s="6">
         <v>2</v>
       </c>
-      <c r="M34" s="106"/>
+      <c r="M34" s="108"/>
       <c r="N34" s="7"/>
       <c r="P34" s="41" t="s">
         <v>65</v>
@@ -6694,7 +6690,7 @@
       <c r="G35" s="3">
         <v>0</v>
       </c>
-      <c r="H35" s="99" t="s">
+      <c r="H35" s="101" t="s">
         <v>15</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -6706,7 +6702,7 @@
       <c r="L35" s="36">
         <v>254</v>
       </c>
-      <c r="M35" s="106"/>
+      <c r="M35" s="108"/>
       <c r="N35" s="37" t="s">
         <v>44</v>
       </c>
@@ -6736,7 +6732,7 @@
       <c r="G36" s="6">
         <v>1</v>
       </c>
-      <c r="H36" s="100"/>
+      <c r="H36" s="102"/>
       <c r="I36" s="7"/>
       <c r="K36" s="11" t="s">
         <v>80</v>
@@ -6744,7 +6740,7 @@
       <c r="L36" s="3">
         <v>255</v>
       </c>
-      <c r="M36" s="106"/>
+      <c r="M36" s="108"/>
       <c r="N36" s="4" t="s">
         <v>19</v>
       </c>
@@ -6774,7 +6770,7 @@
       <c r="G37" s="6">
         <v>2</v>
       </c>
-      <c r="H37" s="100"/>
+      <c r="H37" s="102"/>
       <c r="I37" s="7"/>
       <c r="K37" s="11" t="s">
         <v>81</v>
@@ -6782,7 +6778,7 @@
       <c r="L37" s="3">
         <v>0</v>
       </c>
-      <c r="M37" s="106"/>
+      <c r="M37" s="108"/>
       <c r="N37" s="4" t="s">
         <v>23</v>
       </c>
@@ -6815,7 +6811,7 @@
       <c r="G38" s="6">
         <v>3</v>
       </c>
-      <c r="H38" s="100"/>
+      <c r="H38" s="102"/>
       <c r="I38" s="7"/>
       <c r="K38" s="12" t="s">
         <v>81</v>
@@ -6823,7 +6819,7 @@
       <c r="L38" s="6">
         <v>1</v>
       </c>
-      <c r="M38" s="106"/>
+      <c r="M38" s="108"/>
       <c r="N38" s="7"/>
       <c r="P38" s="77" t="s">
         <v>69</v>
@@ -6852,7 +6848,7 @@
       <c r="G39" s="6">
         <v>4</v>
       </c>
-      <c r="H39" s="100"/>
+      <c r="H39" s="102"/>
       <c r="I39" s="7"/>
       <c r="K39" s="12" t="s">
         <v>81</v>
@@ -6860,7 +6856,7 @@
       <c r="L39" s="6">
         <v>2</v>
       </c>
-      <c r="M39" s="106"/>
+      <c r="M39" s="108"/>
       <c r="N39" s="7"/>
       <c r="P39" s="77" t="s">
         <v>69</v>
@@ -6889,7 +6885,7 @@
       <c r="G40" s="6">
         <v>5</v>
       </c>
-      <c r="H40" s="100"/>
+      <c r="H40" s="102"/>
       <c r="I40" s="7"/>
       <c r="K40" s="35" t="s">
         <v>81</v>
@@ -6897,7 +6893,7 @@
       <c r="L40" s="36">
         <v>254</v>
       </c>
-      <c r="M40" s="106"/>
+      <c r="M40" s="108"/>
       <c r="N40" s="37" t="s">
         <v>44</v>
       </c>
@@ -6928,7 +6924,7 @@
       <c r="G41" s="6">
         <v>6</v>
       </c>
-      <c r="H41" s="100"/>
+      <c r="H41" s="102"/>
       <c r="I41" s="7"/>
       <c r="K41" s="11" t="s">
         <v>81</v>
@@ -6936,7 +6932,7 @@
       <c r="L41" s="3">
         <v>255</v>
       </c>
-      <c r="M41" s="106"/>
+      <c r="M41" s="108"/>
       <c r="N41" s="4" t="s">
         <v>19</v>
       </c>
@@ -6969,7 +6965,7 @@
       <c r="G42" s="6">
         <v>7</v>
       </c>
-      <c r="H42" s="100"/>
+      <c r="H42" s="102"/>
       <c r="I42" s="7"/>
       <c r="K42" s="11" t="s">
         <v>82</v>
@@ -6977,7 +6973,7 @@
       <c r="L42" s="3">
         <v>0</v>
       </c>
-      <c r="M42" s="106"/>
+      <c r="M42" s="108"/>
       <c r="N42" s="4" t="s">
         <v>23</v>
       </c>
@@ -7008,7 +7004,7 @@
       <c r="G43" s="6">
         <v>8</v>
       </c>
-      <c r="H43" s="100"/>
+      <c r="H43" s="102"/>
       <c r="I43" s="7"/>
       <c r="K43" s="12" t="s">
         <v>82</v>
@@ -7016,7 +7012,7 @@
       <c r="L43" s="6">
         <v>1</v>
       </c>
-      <c r="M43" s="106"/>
+      <c r="M43" s="108"/>
       <c r="N43" s="7"/>
       <c r="P43" s="68" t="s">
         <v>69</v>
@@ -7045,7 +7041,7 @@
       <c r="G44" s="6">
         <v>9</v>
       </c>
-      <c r="H44" s="100"/>
+      <c r="H44" s="102"/>
       <c r="I44" s="7"/>
       <c r="K44" s="12" t="s">
         <v>82</v>
@@ -7053,7 +7049,7 @@
       <c r="L44" s="6">
         <v>2</v>
       </c>
-      <c r="M44" s="106"/>
+      <c r="M44" s="108"/>
       <c r="N44" s="7"/>
       <c r="P44" s="70" t="s">
         <v>69</v>
@@ -7082,7 +7078,7 @@
       <c r="G45" s="6">
         <v>10</v>
       </c>
-      <c r="H45" s="100"/>
+      <c r="H45" s="102"/>
       <c r="I45" s="7"/>
       <c r="K45" s="35" t="s">
         <v>82</v>
@@ -7090,7 +7086,7 @@
       <c r="L45" s="36">
         <v>254</v>
       </c>
-      <c r="M45" s="106"/>
+      <c r="M45" s="108"/>
       <c r="N45" s="37" t="s">
         <v>44</v>
       </c>
@@ -7123,7 +7119,7 @@
       <c r="G46" s="33">
         <v>254</v>
       </c>
-      <c r="H46" s="100"/>
+      <c r="H46" s="102"/>
       <c r="I46" s="34" t="s">
         <v>95</v>
       </c>
@@ -7133,7 +7129,7 @@
       <c r="L46" s="3">
         <v>255</v>
       </c>
-      <c r="M46" s="107"/>
+      <c r="M46" s="109"/>
       <c r="N46" s="4" t="s">
         <v>19</v>
       </c>
@@ -7164,7 +7160,7 @@
       <c r="G47" s="3">
         <v>255</v>
       </c>
-      <c r="H47" s="101"/>
+      <c r="H47" s="103"/>
       <c r="I47" s="4" t="s">
         <v>19</v>
       </c>
@@ -7351,7 +7347,7 @@
       <c r="Q56" s="42">
         <v>0</v>
       </c>
-      <c r="R56" s="126" t="s">
+      <c r="R56" s="90" t="s">
         <v>124</v>
       </c>
       <c r="S56" s="4" t="s">
@@ -7376,7 +7372,7 @@
       <c r="Q57" s="41">
         <v>1</v>
       </c>
-      <c r="R57" s="126"/>
+      <c r="R57" s="90"/>
       <c r="S57" s="41" t="s">
         <v>114</v>
       </c>
@@ -7397,7 +7393,7 @@
       <c r="Q58" s="41">
         <v>2</v>
       </c>
-      <c r="R58" s="126"/>
+      <c r="R58" s="90"/>
       <c r="S58" s="41" t="s">
         <v>113</v>
       </c>
@@ -7418,7 +7414,7 @@
       <c r="Q59" s="42">
         <v>3</v>
       </c>
-      <c r="R59" s="126"/>
+      <c r="R59" s="90"/>
       <c r="S59" s="4" t="s">
         <v>19</v>
       </c>
@@ -7449,7 +7445,7 @@
       <c r="Q61" s="78">
         <v>1</v>
       </c>
-      <c r="R61" s="127" t="s">
+      <c r="R61" s="91" t="s">
         <v>125</v>
       </c>
       <c r="S61" s="78" t="s">
@@ -7474,7 +7470,7 @@
       <c r="Q62" s="78">
         <v>2</v>
       </c>
-      <c r="R62" s="127"/>
+      <c r="R62" s="91"/>
       <c r="S62" s="78" t="s">
         <v>66</v>
       </c>
@@ -7498,7 +7494,7 @@
       <c r="Q63" s="72">
         <v>1</v>
       </c>
-      <c r="R63" s="127"/>
+      <c r="R63" s="91"/>
       <c r="S63" s="72" t="s">
         <v>68</v>
       </c>
@@ -7524,7 +7520,7 @@
       <c r="Q64" s="72">
         <v>1</v>
       </c>
-      <c r="R64" s="127"/>
+      <c r="R64" s="91"/>
       <c r="S64" s="72" t="s">
         <v>70</v>
       </c>
@@ -7548,7 +7544,7 @@
       <c r="Q65" s="72">
         <v>2</v>
       </c>
-      <c r="R65" s="127"/>
+      <c r="R65" s="91"/>
       <c r="S65" s="72" t="s">
         <v>71</v>
       </c>
@@ -7572,7 +7568,7 @@
       <c r="Q66" s="72">
         <v>1</v>
       </c>
-      <c r="R66" s="127"/>
+      <c r="R66" s="91"/>
       <c r="S66" s="72" t="s">
         <v>116</v>
       </c>
@@ -8590,7 +8586,7 @@
         <v>40</v>
       </c>
       <c r="G1" s="3"/>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="98" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -8600,7 +8596,7 @@
         <v>87</v>
       </c>
       <c r="L1" s="3"/>
-      <c r="M1" s="114" t="s">
+      <c r="M1" s="116" t="s">
         <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -8610,7 +8606,7 @@
         <v>102</v>
       </c>
       <c r="Q1" s="3"/>
-      <c r="R1" s="108" t="s">
+      <c r="R1" s="110" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -8634,7 +8630,7 @@
         <f>DEC2HEX('ipv4'!G2)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="97"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="66"/>
       <c r="K2" s="12" t="s">
         <v>87</v>
@@ -8643,7 +8639,7 @@
         <f>DEC2HEX('ipv4'!L2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="115"/>
+      <c r="M2" s="117"/>
       <c r="N2" s="66"/>
       <c r="P2" s="12" t="s">
         <v>102</v>
@@ -8652,18 +8648,18 @@
         <f>DEC2HEX('ipv4'!Q2)</f>
         <v>1</v>
       </c>
-      <c r="R2" s="109"/>
+      <c r="R2" s="111"/>
       <c r="S2" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="90" t="s">
+      <c r="AA2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="91"/>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="92"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="94"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -8682,7 +8678,7 @@
         <f>DEC2HEX('ipv4'!G3)</f>
         <v>2</v>
       </c>
-      <c r="H3" s="97"/>
+      <c r="H3" s="99"/>
       <c r="I3" s="66"/>
       <c r="K3" s="12" t="s">
         <v>87</v>
@@ -8691,7 +8687,7 @@
         <f>DEC2HEX('ipv4'!L3)</f>
         <v>2</v>
       </c>
-      <c r="M3" s="115"/>
+      <c r="M3" s="117"/>
       <c r="N3" s="66"/>
       <c r="P3" s="12" t="s">
         <v>102</v>
@@ -8700,7 +8696,7 @@
         <f>DEC2HEX('ipv4'!Q3)</f>
         <v>2</v>
       </c>
-      <c r="R3" s="109"/>
+      <c r="R3" s="111"/>
       <c r="S3" s="66" t="s">
         <v>35</v>
       </c>
@@ -8740,7 +8736,7 @@
         <f>DEC2HEX('ipv4'!G4)</f>
         <v>3</v>
       </c>
-      <c r="H4" s="97"/>
+      <c r="H4" s="99"/>
       <c r="I4" s="66"/>
       <c r="K4" s="12" t="s">
         <v>87</v>
@@ -8749,7 +8745,7 @@
         <f>DEC2HEX('ipv4'!L4)</f>
         <v>3</v>
       </c>
-      <c r="M4" s="115"/>
+      <c r="M4" s="117"/>
       <c r="N4" s="66"/>
       <c r="P4" s="12" t="s">
         <v>102</v>
@@ -8758,7 +8754,7 @@
         <f>DEC2HEX('ipv4'!Q4)</f>
         <v>3</v>
       </c>
-      <c r="R4" s="109"/>
+      <c r="R4" s="111"/>
       <c r="S4" s="66"/>
       <c r="AA4" s="50">
         <v>2001</v>
@@ -8796,7 +8792,7 @@
         <f>DEC2HEX('ipv4'!G5)</f>
         <v>4</v>
       </c>
-      <c r="H5" s="97"/>
+      <c r="H5" s="99"/>
       <c r="I5" s="66"/>
       <c r="K5" s="12" t="s">
         <v>87</v>
@@ -8805,7 +8801,7 @@
         <f>DEC2HEX('ipv4'!L5)</f>
         <v>4</v>
       </c>
-      <c r="M5" s="115"/>
+      <c r="M5" s="117"/>
       <c r="N5" s="66"/>
       <c r="P5" s="12" t="s">
         <v>102</v>
@@ -8814,7 +8810,7 @@
         <f>DEC2HEX('ipv4'!Q5)</f>
         <v>4</v>
       </c>
-      <c r="R5" s="109"/>
+      <c r="R5" s="111"/>
       <c r="S5" s="66"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -8834,13 +8830,13 @@
         <f>DEC2HEX('ipv4'!G6)</f>
         <v>5</v>
       </c>
-      <c r="H6" s="97"/>
+      <c r="H6" s="99"/>
       <c r="I6" s="66"/>
       <c r="K6" s="11" t="s">
         <v>96</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="115"/>
+      <c r="M6" s="117"/>
       <c r="N6" s="4" t="s">
         <v>23</v>
       </c>
@@ -8848,14 +8844,14 @@
         <v>103</v>
       </c>
       <c r="Q6" s="60"/>
-      <c r="R6" s="109"/>
+      <c r="R6" s="111"/>
       <c r="S6" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="AA6" s="94" t="s">
+      <c r="AA6" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="95"/>
+      <c r="AB6" s="97"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -8874,7 +8870,7 @@
         <f>DEC2HEX('ipv4'!G7)</f>
         <v>6</v>
       </c>
-      <c r="H7" s="97"/>
+      <c r="H7" s="99"/>
       <c r="I7" s="66"/>
       <c r="K7" s="12" t="s">
         <v>96</v>
@@ -8883,7 +8879,7 @@
         <f>DEC2HEX('ipv4'!L9)</f>
         <v>1</v>
       </c>
-      <c r="M7" s="115"/>
+      <c r="M7" s="117"/>
       <c r="N7" s="66"/>
       <c r="P7" s="12" t="s">
         <v>103</v>
@@ -8892,7 +8888,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R7" s="109"/>
+      <c r="R7" s="111"/>
       <c r="S7" s="66"/>
       <c r="AA7" s="48" t="s">
         <v>42</v>
@@ -8918,7 +8914,7 @@
         <f>DEC2HEX('ipv4'!G8)</f>
         <v>7</v>
       </c>
-      <c r="H8" s="97"/>
+      <c r="H8" s="99"/>
       <c r="I8" s="66"/>
       <c r="K8" s="12" t="s">
         <v>96</v>
@@ -8927,7 +8923,7 @@
         <f>DEC2HEX('ipv4'!L10)</f>
         <v>2</v>
       </c>
-      <c r="M8" s="115"/>
+      <c r="M8" s="117"/>
       <c r="N8" s="66"/>
       <c r="P8" s="12" t="s">
         <v>103</v>
@@ -8936,7 +8932,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R8" s="109"/>
+      <c r="R8" s="111"/>
       <c r="S8" s="66"/>
       <c r="AA8" s="48" t="s">
         <v>43</v>
@@ -8962,7 +8958,7 @@
         <f>DEC2HEX('ipv4'!G9)</f>
         <v>8</v>
       </c>
-      <c r="H9" s="97"/>
+      <c r="H9" s="99"/>
       <c r="I9" s="66"/>
       <c r="K9" s="12" t="s">
         <v>96</v>
@@ -8971,13 +8967,13 @@
         <f>DEC2HEX('ipv4'!L11)</f>
         <v>3</v>
       </c>
-      <c r="M9" s="115"/>
+      <c r="M9" s="117"/>
       <c r="N9" s="66"/>
       <c r="P9" s="59" t="s">
         <v>104</v>
       </c>
       <c r="Q9" s="60"/>
-      <c r="R9" s="109"/>
+      <c r="R9" s="111"/>
       <c r="S9" s="61" t="s">
         <v>23</v>
       </c>
@@ -9005,7 +9001,7 @@
         <f>DEC2HEX('ipv4'!G10)</f>
         <v>9</v>
       </c>
-      <c r="H10" s="97"/>
+      <c r="H10" s="99"/>
       <c r="I10" s="66"/>
       <c r="K10" s="12" t="s">
         <v>96</v>
@@ -9014,7 +9010,7 @@
         <f>DEC2HEX('ipv4'!L12)</f>
         <v>4</v>
       </c>
-      <c r="M10" s="115"/>
+      <c r="M10" s="117"/>
       <c r="N10" s="66"/>
       <c r="P10" s="12" t="s">
         <v>104</v>
@@ -9023,7 +9019,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R10" s="109"/>
+      <c r="R10" s="111"/>
       <c r="S10" s="66"/>
       <c r="AA10" s="49" t="s">
         <v>85</v>
@@ -9049,13 +9045,13 @@
         <f>DEC2HEX('ipv4'!G11)</f>
         <v>A</v>
       </c>
-      <c r="H11" s="97"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="66"/>
       <c r="K11" s="11" t="s">
         <v>97</v>
       </c>
       <c r="L11" s="3"/>
-      <c r="M11" s="115"/>
+      <c r="M11" s="117"/>
       <c r="N11" s="4" t="s">
         <v>23</v>
       </c>
@@ -9066,7 +9062,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R11" s="109"/>
+      <c r="R11" s="111"/>
       <c r="S11" s="66"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
@@ -9086,7 +9082,7 @@
         <f>DEC2HEX('ipv4'!G12)</f>
         <v>B</v>
       </c>
-      <c r="H12" s="97"/>
+      <c r="H12" s="99"/>
       <c r="I12" s="66"/>
       <c r="K12" s="12" t="s">
         <v>97</v>
@@ -9095,13 +9091,13 @@
         <f>DEC2HEX('ipv4'!L16)</f>
         <v>1</v>
       </c>
-      <c r="M12" s="115"/>
+      <c r="M12" s="117"/>
       <c r="N12" s="66"/>
       <c r="P12" s="59" t="s">
         <v>105</v>
       </c>
       <c r="Q12" s="60"/>
-      <c r="R12" s="109"/>
+      <c r="R12" s="111"/>
       <c r="S12" s="61" t="s">
         <v>23</v>
       </c>
@@ -9127,7 +9123,7 @@
         <f>DEC2HEX('ipv4'!G13)</f>
         <v>C</v>
       </c>
-      <c r="H13" s="97"/>
+      <c r="H13" s="99"/>
       <c r="I13" s="66"/>
       <c r="K13" s="12" t="s">
         <v>97</v>
@@ -9136,7 +9132,7 @@
         <f>DEC2HEX('ipv4'!L17)</f>
         <v>2</v>
       </c>
-      <c r="M13" s="115"/>
+      <c r="M13" s="117"/>
       <c r="N13" s="66"/>
       <c r="P13" s="12" t="s">
         <v>105</v>
@@ -9145,7 +9141,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R13" s="109"/>
+      <c r="R13" s="111"/>
       <c r="S13" s="66"/>
       <c r="AA13" s="45"/>
       <c r="AB13" s="46"/>
@@ -9169,7 +9165,7 @@
         <f>DEC2HEX('ipv4'!G14)</f>
         <v>D</v>
       </c>
-      <c r="H14" s="97"/>
+      <c r="H14" s="99"/>
       <c r="I14" s="66"/>
       <c r="K14" s="12" t="s">
         <v>97</v>
@@ -9178,7 +9174,7 @@
         <f>DEC2HEX('ipv4'!L18)</f>
         <v>3</v>
       </c>
-      <c r="M14" s="115"/>
+      <c r="M14" s="117"/>
       <c r="N14" s="66"/>
       <c r="P14" s="12" t="s">
         <v>105</v>
@@ -9187,7 +9183,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R14" s="110"/>
+      <c r="R14" s="112"/>
       <c r="S14" s="66"/>
       <c r="AA14" s="47"/>
       <c r="AB14" s="47"/>
@@ -9211,7 +9207,7 @@
         <f>DEC2HEX('ipv4'!G15)</f>
         <v>E</v>
       </c>
-      <c r="H15" s="97"/>
+      <c r="H15" s="99"/>
       <c r="I15" s="66"/>
       <c r="K15" s="12" t="s">
         <v>97</v>
@@ -9220,13 +9216,13 @@
         <f>DEC2HEX('ipv4'!L19)</f>
         <v>4</v>
       </c>
-      <c r="M15" s="116"/>
+      <c r="M15" s="118"/>
       <c r="N15" s="66"/>
       <c r="P15" s="59" t="s">
         <v>106</v>
       </c>
       <c r="Q15" s="60"/>
-      <c r="R15" s="109" t="s">
+      <c r="R15" s="111" t="s">
         <v>20</v>
       </c>
       <c r="S15" s="61" t="s">
@@ -9254,7 +9250,7 @@
         <f>DEC2HEX('ipv4'!G16)</f>
         <v>F</v>
       </c>
-      <c r="H16" s="97"/>
+      <c r="H16" s="99"/>
       <c r="I16" s="66"/>
       <c r="M16" s="38"/>
       <c r="P16" s="12" t="s">
@@ -9264,7 +9260,7 @@
         <f>DEC2HEX('ipv4'!Q10)</f>
         <v>1</v>
       </c>
-      <c r="R16" s="109"/>
+      <c r="R16" s="111"/>
       <c r="S16" s="66" t="s">
         <v>21</v>
       </c>
@@ -9290,13 +9286,13 @@
         <f>DEC2HEX('ipv4'!G17)</f>
         <v>10</v>
       </c>
-      <c r="H17" s="97"/>
+      <c r="H17" s="99"/>
       <c r="I17" s="66"/>
       <c r="K17" s="11" t="s">
         <v>98</v>
       </c>
       <c r="L17" s="3"/>
-      <c r="M17" s="120" t="s">
+      <c r="M17" s="122" t="s">
         <v>16</v>
       </c>
       <c r="N17" s="4" t="s">
@@ -9309,7 +9305,7 @@
         <f>DEC2HEX('ipv4'!Q11)</f>
         <v>2</v>
       </c>
-      <c r="R17" s="110"/>
+      <c r="R17" s="112"/>
       <c r="S17" s="66" t="s">
         <v>22</v>
       </c>
@@ -9335,7 +9331,7 @@
         <f>DEC2HEX('ipv4'!G18)</f>
         <v>11</v>
       </c>
-      <c r="H18" s="97"/>
+      <c r="H18" s="99"/>
       <c r="I18" s="66"/>
       <c r="K18" s="12" t="s">
         <v>98</v>
@@ -9344,7 +9340,7 @@
         <f>DEC2HEX('ipv4'!L24)</f>
         <v>1</v>
       </c>
-      <c r="M18" s="121"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="66"/>
       <c r="R18" s="62"/>
       <c r="AA18" s="29"/>
@@ -9369,7 +9365,7 @@
         <f>DEC2HEX('ipv4'!G19)</f>
         <v>12</v>
       </c>
-      <c r="H19" s="97"/>
+      <c r="H19" s="99"/>
       <c r="I19" s="66"/>
       <c r="K19" s="12" t="s">
         <v>98</v>
@@ -9378,13 +9374,13 @@
         <f>DEC2HEX('ipv4'!L25)</f>
         <v>2</v>
       </c>
-      <c r="M19" s="121"/>
+      <c r="M19" s="123"/>
       <c r="N19" s="66"/>
       <c r="P19" s="64" t="s">
         <v>108</v>
       </c>
       <c r="Q19" s="42"/>
-      <c r="R19" s="111" t="s">
+      <c r="R19" s="113" t="s">
         <v>73</v>
       </c>
       <c r="S19" s="4" t="s">
@@ -9412,7 +9408,7 @@
         <f>DEC2HEX('ipv4'!G20)</f>
         <v>13</v>
       </c>
-      <c r="H20" s="97"/>
+      <c r="H20" s="99"/>
       <c r="I20" s="66"/>
       <c r="K20" s="12" t="s">
         <v>98</v>
@@ -9421,7 +9417,7 @@
         <f>DEC2HEX('ipv4'!L26)</f>
         <v>3</v>
       </c>
-      <c r="M20" s="121"/>
+      <c r="M20" s="123"/>
       <c r="N20" s="66"/>
       <c r="P20" s="65" t="s">
         <v>108</v>
@@ -9430,7 +9426,7 @@
         <f>DEC2HEX('ipv4'!Q16)</f>
         <v>1</v>
       </c>
-      <c r="R20" s="112"/>
+      <c r="R20" s="114"/>
       <c r="S20" s="41" t="s">
         <v>67</v>
       </c>
@@ -9456,7 +9452,7 @@
         <f>DEC2HEX('ipv4'!G21)</f>
         <v>14</v>
       </c>
-      <c r="H21" s="97"/>
+      <c r="H21" s="99"/>
       <c r="I21" s="66"/>
       <c r="K21" s="12" t="s">
         <v>98</v>
@@ -9465,7 +9461,7 @@
         <f>DEC2HEX('ipv4'!L27)</f>
         <v>4</v>
       </c>
-      <c r="M21" s="121"/>
+      <c r="M21" s="123"/>
       <c r="N21" s="66"/>
       <c r="P21" s="65" t="s">
         <v>108</v>
@@ -9474,7 +9470,7 @@
         <f>DEC2HEX('ipv4'!Q17)</f>
         <v>2</v>
       </c>
-      <c r="R21" s="112"/>
+      <c r="R21" s="114"/>
       <c r="S21" s="41" t="s">
         <v>66</v>
       </c>
@@ -9500,7 +9496,7 @@
         <f>DEC2HEX('ipv4'!G22)</f>
         <v>15</v>
       </c>
-      <c r="H22" s="97"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="66"/>
       <c r="K22" s="12" t="s">
         <v>98</v>
@@ -9509,7 +9505,7 @@
         <f>DEC2HEX('ipv4'!L28)</f>
         <v>5</v>
       </c>
-      <c r="M22" s="122"/>
+      <c r="M22" s="124"/>
       <c r="N22" s="66"/>
       <c r="P22" s="65" t="s">
         <v>108</v>
@@ -9518,7 +9514,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R22" s="112"/>
+      <c r="R22" s="114"/>
       <c r="S22" s="41" t="s">
         <v>51</v>
       </c>
@@ -9544,7 +9540,7 @@
         <f>DEC2HEX('ipv4'!G23)</f>
         <v>16</v>
       </c>
-      <c r="H23" s="97"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="66"/>
       <c r="M23" s="58"/>
       <c r="P23" s="65" t="s">
@@ -9554,7 +9550,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R23" s="112"/>
+      <c r="R23" s="114"/>
       <c r="S23" s="41" t="s">
         <v>52</v>
       </c>
@@ -9580,13 +9576,13 @@
         <f>DEC2HEX('ipv4'!G24)</f>
         <v>17</v>
       </c>
-      <c r="H24" s="97"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="66"/>
       <c r="K24" s="11" t="s">
         <v>99</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="123" t="s">
+      <c r="M24" s="125" t="s">
         <v>24</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -9597,9 +9593,9 @@
       </c>
       <c r="Q24" s="41" t="str">
         <f>DEC2HEX('ipv4'!Q21)</f>
-        <v>A</v>
-      </c>
-      <c r="R24" s="112"/>
+        <v>6</v>
+      </c>
+      <c r="R24" s="114"/>
       <c r="S24" s="41" t="s">
         <v>53</v>
       </c>
@@ -9625,7 +9621,7 @@
         <f>DEC2HEX('ipv4'!G25)</f>
         <v>18</v>
       </c>
-      <c r="H25" s="97"/>
+      <c r="H25" s="99"/>
       <c r="I25" s="66"/>
       <c r="K25" s="12" t="s">
         <v>99</v>
@@ -9634,16 +9630,16 @@
         <f>DEC2HEX('ipv4'!L33)</f>
         <v>1</v>
       </c>
-      <c r="M25" s="124"/>
+      <c r="M25" s="126"/>
       <c r="N25" s="66"/>
       <c r="P25" s="65" t="s">
         <v>108</v>
       </c>
       <c r="Q25" s="41" t="str">
         <f>DEC2HEX('ipv4'!Q24)</f>
-        <v>D</v>
-      </c>
-      <c r="R25" s="112"/>
+        <v>9</v>
+      </c>
+      <c r="R25" s="114"/>
       <c r="S25" s="41" t="s">
         <v>58</v>
       </c>
@@ -9665,7 +9661,7 @@
         <f>DEC2HEX('ipv4'!G26)</f>
         <v>19</v>
       </c>
-      <c r="H26" s="97"/>
+      <c r="H26" s="99"/>
       <c r="I26" s="66"/>
       <c r="K26" s="12" t="s">
         <v>99</v>
@@ -9674,16 +9670,16 @@
         <f>DEC2HEX('ipv4'!L34)</f>
         <v>2</v>
       </c>
-      <c r="M26" s="124"/>
+      <c r="M26" s="126"/>
       <c r="N26" s="67"/>
       <c r="P26" s="65" t="s">
         <v>108</v>
       </c>
       <c r="Q26" s="41" t="str">
         <f>DEC2HEX('ipv4'!Q25)</f>
-        <v>E</v>
-      </c>
-      <c r="R26" s="112"/>
+        <v>A</v>
+      </c>
+      <c r="R26" s="114"/>
       <c r="S26" s="41" t="s">
         <v>59</v>
       </c>
@@ -9705,13 +9701,13 @@
         <f>DEC2HEX('ipv4'!G27)</f>
         <v>1A</v>
       </c>
-      <c r="H27" s="97"/>
+      <c r="H27" s="99"/>
       <c r="I27" s="66"/>
       <c r="K27" s="11" t="s">
         <v>100</v>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="124"/>
+      <c r="M27" s="126"/>
       <c r="N27" s="4" t="s">
         <v>23</v>
       </c>
@@ -9720,9 +9716,9 @@
       </c>
       <c r="Q27" s="41" t="str">
         <f>DEC2HEX('ipv4'!Q26)</f>
-        <v>F</v>
-      </c>
-      <c r="R27" s="112"/>
+        <v>B</v>
+      </c>
+      <c r="R27" s="114"/>
       <c r="S27" s="41" t="s">
         <v>60</v>
       </c>
@@ -9744,7 +9740,7 @@
         <f>DEC2HEX('ipv4'!G28)</f>
         <v>1B</v>
       </c>
-      <c r="H28" s="97"/>
+      <c r="H28" s="99"/>
       <c r="I28" s="66"/>
       <c r="K28" s="12" t="s">
         <v>100</v>
@@ -9753,13 +9749,13 @@
         <f>DEC2HEX('ipv4'!L38)</f>
         <v>1</v>
       </c>
-      <c r="M28" s="124"/>
+      <c r="M28" s="126"/>
       <c r="N28" s="66"/>
       <c r="P28" s="64" t="s">
         <v>109</v>
       </c>
       <c r="Q28" s="42"/>
-      <c r="R28" s="112"/>
+      <c r="R28" s="114"/>
       <c r="S28" s="4" t="s">
         <v>23</v>
       </c>
@@ -9781,7 +9777,7 @@
         <f>DEC2HEX('ipv4'!G29)</f>
         <v>1C</v>
       </c>
-      <c r="H29" s="97"/>
+      <c r="H29" s="99"/>
       <c r="I29" s="66"/>
       <c r="K29" s="12" t="s">
         <v>100</v>
@@ -9790,7 +9786,7 @@
         <f>DEC2HEX('ipv4'!L39)</f>
         <v>2</v>
       </c>
-      <c r="M29" s="124"/>
+      <c r="M29" s="126"/>
       <c r="N29" s="66"/>
       <c r="P29" s="65" t="s">
         <v>109</v>
@@ -9799,7 +9795,7 @@
         <f>DEC2HEX('ipv4'!Q32)</f>
         <v>1</v>
       </c>
-      <c r="R29" s="112"/>
+      <c r="R29" s="114"/>
       <c r="S29" s="41" t="s">
         <v>68</v>
       </c>
@@ -9821,13 +9817,13 @@
         <f>DEC2HEX('ipv4'!G30)</f>
         <v>1D</v>
       </c>
-      <c r="H30" s="97"/>
+      <c r="H30" s="99"/>
       <c r="I30" s="66"/>
       <c r="K30" s="59" t="s">
         <v>101</v>
       </c>
       <c r="L30" s="60"/>
-      <c r="M30" s="124"/>
+      <c r="M30" s="126"/>
       <c r="N30" s="61" t="s">
         <v>23</v>
       </c>
@@ -9838,7 +9834,7 @@
         <f>DEC2HEX('ipv4'!Q33)</f>
         <v>2</v>
       </c>
-      <c r="R30" s="112"/>
+      <c r="R30" s="114"/>
       <c r="S30" s="41" t="s">
         <v>45</v>
       </c>
@@ -9860,7 +9856,7 @@
         <f>DEC2HEX('ipv4'!G31)</f>
         <v>1E</v>
       </c>
-      <c r="H31" s="98"/>
+      <c r="H31" s="100"/>
       <c r="I31" s="66"/>
       <c r="K31" s="12" t="s">
         <v>101</v>
@@ -9869,7 +9865,7 @@
         <f>DEC2HEX('ipv4'!L43)</f>
         <v>1</v>
       </c>
-      <c r="M31" s="124"/>
+      <c r="M31" s="126"/>
       <c r="N31" s="66"/>
       <c r="P31" s="65" t="s">
         <v>109</v>
@@ -9878,7 +9874,7 @@
         <f>DEC2HEX('ipv4'!Q34)</f>
         <v>3</v>
       </c>
-      <c r="R31" s="112"/>
+      <c r="R31" s="114"/>
       <c r="S31" s="41" t="s">
         <v>54</v>
       </c>
@@ -9904,13 +9900,13 @@
         <f>DEC2HEX('ipv4'!L44)</f>
         <v>2</v>
       </c>
-      <c r="M32" s="125"/>
+      <c r="M32" s="127"/>
       <c r="N32" s="66"/>
       <c r="P32" s="64" t="s">
         <v>110</v>
       </c>
       <c r="Q32" s="42"/>
-      <c r="R32" s="112"/>
+      <c r="R32" s="114"/>
       <c r="S32" s="4" t="s">
         <v>23</v>
       </c>
@@ -9929,7 +9925,7 @@
         <v>86</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="117" t="s">
+      <c r="H33" s="119" t="s">
         <v>15</v>
       </c>
       <c r="I33" s="4" t="s">
@@ -9946,7 +9942,7 @@
         <f>DEC2HEX('ipv4'!Q38)</f>
         <v>1</v>
       </c>
-      <c r="R33" s="112"/>
+      <c r="R33" s="114"/>
       <c r="S33" s="41" t="s">
         <v>70</v>
       </c>
@@ -9968,7 +9964,7 @@
         <f>DEC2HEX('ipv4'!G36)</f>
         <v>1</v>
       </c>
-      <c r="H34" s="118"/>
+      <c r="H34" s="120"/>
       <c r="I34" s="66"/>
       <c r="P34" s="65" t="s">
         <v>110</v>
@@ -9977,7 +9973,7 @@
         <f>DEC2HEX('ipv4'!Q39)</f>
         <v>2</v>
       </c>
-      <c r="R34" s="112"/>
+      <c r="R34" s="114"/>
       <c r="S34" s="41" t="s">
         <v>71</v>
       </c>
@@ -9999,7 +9995,7 @@
         <f>DEC2HEX('ipv4'!G37)</f>
         <v>2</v>
       </c>
-      <c r="H35" s="118"/>
+      <c r="H35" s="120"/>
       <c r="I35" s="66"/>
       <c r="P35" s="65" t="s">
         <v>110</v>
@@ -10008,7 +10004,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R35" s="112"/>
+      <c r="R35" s="114"/>
       <c r="S35" s="41" t="s">
         <v>47</v>
       </c>
@@ -10030,7 +10026,7 @@
         <f>DEC2HEX('ipv4'!G38)</f>
         <v>3</v>
       </c>
-      <c r="H36" s="118"/>
+      <c r="H36" s="120"/>
       <c r="I36" s="66"/>
       <c r="P36" s="65" t="s">
         <v>110</v>
@@ -10039,7 +10035,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R36" s="112"/>
+      <c r="R36" s="114"/>
       <c r="S36" s="41" t="s">
         <v>48</v>
       </c>
@@ -10061,7 +10057,7 @@
         <f>DEC2HEX('ipv4'!G39)</f>
         <v>4</v>
       </c>
-      <c r="H37" s="118"/>
+      <c r="H37" s="120"/>
       <c r="I37" s="66"/>
       <c r="P37" s="65" t="s">
         <v>110</v>
@@ -10070,7 +10066,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R37" s="112"/>
+      <c r="R37" s="114"/>
       <c r="S37" s="41" t="s">
         <v>49</v>
       </c>
@@ -10092,7 +10088,7 @@
         <f>DEC2HEX('ipv4'!G40)</f>
         <v>5</v>
       </c>
-      <c r="H38" s="118"/>
+      <c r="H38" s="120"/>
       <c r="I38" s="66"/>
       <c r="P38" s="65" t="s">
         <v>110</v>
@@ -10101,7 +10097,7 @@
         <f>DEC2HEX('ipv4'!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R38" s="112"/>
+      <c r="R38" s="114"/>
       <c r="S38" s="41" t="s">
         <v>50</v>
       </c>
@@ -10123,7 +10119,7 @@
         <f>DEC2HEX('ipv4'!G41)</f>
         <v>6</v>
       </c>
-      <c r="H39" s="118"/>
+      <c r="H39" s="120"/>
       <c r="I39" s="66"/>
       <c r="P39" s="65" t="s">
         <v>110</v>
@@ -10132,7 +10128,7 @@
         <f>DEC2HEX('ipv4'!Q40)</f>
         <v>3</v>
       </c>
-      <c r="R39" s="112"/>
+      <c r="R39" s="114"/>
       <c r="S39" s="41" t="s">
         <v>57</v>
       </c>
@@ -10154,7 +10150,7 @@
         <f>DEC2HEX('ipv4'!G42)</f>
         <v>7</v>
       </c>
-      <c r="H40" s="118"/>
+      <c r="H40" s="120"/>
       <c r="I40" s="66"/>
       <c r="P40" s="65" t="s">
         <v>110</v>
@@ -10163,7 +10159,7 @@
         <f>DEC2HEX('ipv4'!Q41)</f>
         <v>4</v>
       </c>
-      <c r="R40" s="112"/>
+      <c r="R40" s="114"/>
       <c r="S40" s="41" t="s">
         <v>56</v>
       </c>
@@ -10185,13 +10181,13 @@
         <f>DEC2HEX('ipv4'!G43)</f>
         <v>8</v>
       </c>
-      <c r="H41" s="118"/>
+      <c r="H41" s="120"/>
       <c r="I41" s="66"/>
       <c r="P41" s="64" t="s">
         <v>111</v>
       </c>
       <c r="Q41" s="42"/>
-      <c r="R41" s="112"/>
+      <c r="R41" s="114"/>
       <c r="S41" s="4" t="s">
         <v>23</v>
       </c>
@@ -10213,7 +10209,7 @@
         <f>DEC2HEX('ipv4'!G44)</f>
         <v>9</v>
       </c>
-      <c r="H42" s="118"/>
+      <c r="H42" s="120"/>
       <c r="I42" s="66"/>
       <c r="P42" s="65" t="s">
         <v>111</v>
@@ -10222,7 +10218,7 @@
         <f>DEC2HEX('ipv4'!Q50)</f>
         <v>1</v>
       </c>
-      <c r="R42" s="112"/>
+      <c r="R42" s="114"/>
       <c r="S42" s="41" t="s">
         <v>46</v>
       </c>
@@ -10244,7 +10240,7 @@
         <f>DEC2HEX('ipv4'!G45)</f>
         <v>A</v>
       </c>
-      <c r="H43" s="119"/>
+      <c r="H43" s="121"/>
       <c r="I43" s="66"/>
       <c r="P43" s="65" t="s">
         <v>111</v>
@@ -10253,7 +10249,7 @@
         <f>DEC2HEX('ipv4'!Q51)</f>
         <v>2</v>
       </c>
-      <c r="R43" s="113"/>
+      <c r="R43" s="115"/>
       <c r="S43" s="41" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
todolist es probalkozasok hsrp-re, eddig sikertelenul
</commit_message>
<xml_diff>
--- a/Documentations/VLANs/VLSM-tablazat.xlsx
+++ b/Documentations/VLANs/VLSM-tablazat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doboz\Desktop\aromas-cubanos\Documentations\VLANs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\aromas-cubanos\Documentations\VLANs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C063EA-1CD1-4EE6-A651-5795D14142D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76C0E8A-D68D-48B1-AE24-D8DF1784ED8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5295" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{012D1D82-EB97-4B95-AC21-450975C8649A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{012D1D82-EB97-4B95-AC21-450975C8649A}"/>
   </bookViews>
   <sheets>
     <sheet name="plain" sheetId="1" r:id="rId1"/>
@@ -22,23 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="125">
   <si>
     <t>/30</t>
   </si>
@@ -407,6 +396,12 @@
   </si>
   <si>
     <t>2001:db8:1984::</t>
+  </si>
+  <si>
+    <t>RF Virtual GW</t>
+  </si>
+  <si>
+    <t>RV Virtual GW</t>
   </si>
 </sst>
 </file>
@@ -613,7 +608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -869,12 +864,27 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1026,15 +1036,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,33 +1099,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1161,6 +1135,55 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Jó" xfId="1" builtinId="26"/>
@@ -1170,10 +1193,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD9E1F2"/>
       <color rgb="FFE7FE5E"/>
       <color rgb="FFF36969"/>
       <color rgb="FFF03E3E"/>
-      <color rgb="FFD9E1F2"/>
       <color rgb="FFFFB9B9"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFFFF66"/>
@@ -1191,9 +1214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1231,7 +1254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1337,7 +1360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1479,7 +1502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5051,52 +5074,61 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="C86:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="C134:C137"/>
-    <mergeCell ref="C138:C141"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C178:C181"/>
-    <mergeCell ref="C182:C185"/>
-    <mergeCell ref="C186:C189"/>
-    <mergeCell ref="C190:C193"/>
-    <mergeCell ref="C146:C149"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="C158:C161"/>
-    <mergeCell ref="C162:C165"/>
-    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="H2:H129"/>
+    <mergeCell ref="H130:H257"/>
+    <mergeCell ref="F162:F193"/>
+    <mergeCell ref="F194:F225"/>
+    <mergeCell ref="F226:F257"/>
+    <mergeCell ref="G2:G65"/>
+    <mergeCell ref="G66:G129"/>
+    <mergeCell ref="G130:G193"/>
+    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="E178:E193"/>
+    <mergeCell ref="E194:E209"/>
+    <mergeCell ref="E210:E225"/>
+    <mergeCell ref="E226:E241"/>
+    <mergeCell ref="E242:E257"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="F34:F65"/>
+    <mergeCell ref="F66:F97"/>
+    <mergeCell ref="F98:F129"/>
+    <mergeCell ref="F130:F161"/>
+    <mergeCell ref="E82:E97"/>
+    <mergeCell ref="E98:E113"/>
+    <mergeCell ref="E114:E129"/>
+    <mergeCell ref="E130:E145"/>
+    <mergeCell ref="E146:E161"/>
+    <mergeCell ref="E162:E177"/>
+    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="E34:E49"/>
+    <mergeCell ref="E50:E65"/>
+    <mergeCell ref="E66:E81"/>
+    <mergeCell ref="D242:D249"/>
+    <mergeCell ref="D250:D257"/>
+    <mergeCell ref="D194:D201"/>
+    <mergeCell ref="D202:D209"/>
+    <mergeCell ref="D210:D217"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="D226:D233"/>
+    <mergeCell ref="D234:D241"/>
+    <mergeCell ref="D146:D153"/>
+    <mergeCell ref="D154:D161"/>
+    <mergeCell ref="D162:D169"/>
+    <mergeCell ref="D170:D177"/>
+    <mergeCell ref="D178:D185"/>
+    <mergeCell ref="D186:D193"/>
+    <mergeCell ref="D106:D113"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="D122:D129"/>
+    <mergeCell ref="D130:D137"/>
+    <mergeCell ref="D138:D145"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="D82:D89"/>
+    <mergeCell ref="D90:D97"/>
     <mergeCell ref="C242:C245"/>
     <mergeCell ref="C246:C249"/>
     <mergeCell ref="C250:C253"/>
@@ -5121,61 +5153,52 @@
     <mergeCell ref="C170:C173"/>
     <mergeCell ref="C174:C177"/>
     <mergeCell ref="D98:D105"/>
-    <mergeCell ref="D106:D113"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="D122:D129"/>
-    <mergeCell ref="D130:D137"/>
-    <mergeCell ref="D138:D145"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="D82:D89"/>
-    <mergeCell ref="D90:D97"/>
-    <mergeCell ref="D242:D249"/>
-    <mergeCell ref="D250:D257"/>
-    <mergeCell ref="D194:D201"/>
-    <mergeCell ref="D202:D209"/>
-    <mergeCell ref="D210:D217"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="D226:D233"/>
-    <mergeCell ref="D234:D241"/>
-    <mergeCell ref="D146:D153"/>
-    <mergeCell ref="D154:D161"/>
-    <mergeCell ref="D162:D169"/>
-    <mergeCell ref="D170:D177"/>
-    <mergeCell ref="D178:D185"/>
-    <mergeCell ref="D186:D193"/>
-    <mergeCell ref="E178:E193"/>
-    <mergeCell ref="E194:E209"/>
-    <mergeCell ref="E210:E225"/>
-    <mergeCell ref="E226:E241"/>
-    <mergeCell ref="E242:E257"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="F34:F65"/>
-    <mergeCell ref="F66:F97"/>
-    <mergeCell ref="F98:F129"/>
-    <mergeCell ref="F130:F161"/>
-    <mergeCell ref="E82:E97"/>
-    <mergeCell ref="E98:E113"/>
-    <mergeCell ref="E114:E129"/>
-    <mergeCell ref="E130:E145"/>
-    <mergeCell ref="E146:E161"/>
-    <mergeCell ref="E162:E177"/>
-    <mergeCell ref="E2:E17"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="E34:E49"/>
-    <mergeCell ref="E50:E65"/>
-    <mergeCell ref="E66:E81"/>
-    <mergeCell ref="H2:H129"/>
-    <mergeCell ref="H130:H257"/>
-    <mergeCell ref="F162:F193"/>
-    <mergeCell ref="F194:F225"/>
-    <mergeCell ref="F226:F257"/>
-    <mergeCell ref="G2:G65"/>
-    <mergeCell ref="G66:G129"/>
-    <mergeCell ref="G130:G193"/>
-    <mergeCell ref="G194:G257"/>
+    <mergeCell ref="C178:C181"/>
+    <mergeCell ref="C182:C185"/>
+    <mergeCell ref="C186:C189"/>
+    <mergeCell ref="C190:C193"/>
+    <mergeCell ref="C146:C149"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="C158:C161"/>
+    <mergeCell ref="C162:C165"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -5186,8 +5209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709A4C10-0955-4D97-86D1-D5085866A222}">
   <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7:AB10"/>
+    <sheetView tabSelected="1" topLeftCell="J34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB42" sqref="AB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5241,7 +5264,7 @@
       <c r="G1" s="3">
         <v>0</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="81" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -5253,7 +5276,7 @@
       <c r="L1" s="3">
         <v>0</v>
       </c>
-      <c r="M1" s="90" t="s">
+      <c r="M1" s="87" t="s">
         <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -5265,7 +5288,7 @@
       <c r="Q1" s="33">
         <v>0</v>
       </c>
-      <c r="R1" s="96" t="s">
+      <c r="R1" s="93" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -5287,7 +5310,7 @@
       <c r="G2" s="6">
         <v>1</v>
       </c>
-      <c r="H2" s="85"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="7"/>
       <c r="K2" s="10" t="s">
         <v>74</v>
@@ -5295,7 +5318,7 @@
       <c r="L2" s="6">
         <v>1</v>
       </c>
-      <c r="M2" s="91"/>
+      <c r="M2" s="88"/>
       <c r="N2" s="7"/>
       <c r="P2" s="10" t="s">
         <v>81</v>
@@ -5303,16 +5326,16 @@
       <c r="Q2" s="32">
         <v>1</v>
       </c>
-      <c r="R2" s="97"/>
+      <c r="R2" s="94"/>
       <c r="S2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="78" t="s">
+      <c r="AA2" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
-      <c r="AD2" s="80"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="77"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -5329,7 +5352,7 @@
       <c r="G3" s="6">
         <v>2</v>
       </c>
-      <c r="H3" s="85"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="7"/>
       <c r="K3" s="10" t="s">
         <v>74</v>
@@ -5337,7 +5360,7 @@
       <c r="L3" s="6">
         <v>2</v>
       </c>
-      <c r="M3" s="91"/>
+      <c r="M3" s="88"/>
       <c r="N3" s="7"/>
       <c r="P3" s="10" t="s">
         <v>81</v>
@@ -5345,7 +5368,7 @@
       <c r="Q3" s="32">
         <v>2</v>
       </c>
-      <c r="R3" s="97"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="7" t="s">
         <v>33</v>
       </c>
@@ -5377,7 +5400,7 @@
       <c r="G4" s="6">
         <v>3</v>
       </c>
-      <c r="H4" s="85"/>
+      <c r="H4" s="82"/>
       <c r="I4" s="7"/>
       <c r="K4" s="10" t="s">
         <v>74</v>
@@ -5385,7 +5408,7 @@
       <c r="L4" s="6">
         <v>3</v>
       </c>
-      <c r="M4" s="91"/>
+      <c r="M4" s="88"/>
       <c r="N4" s="7"/>
       <c r="P4" s="10" t="s">
         <v>81</v>
@@ -5393,7 +5416,7 @@
       <c r="Q4" s="32">
         <v>3</v>
       </c>
-      <c r="R4" s="97"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="7"/>
       <c r="AA4" s="18">
         <v>10</v>
@@ -5423,7 +5446,7 @@
       <c r="G5" s="6">
         <v>4</v>
       </c>
-      <c r="H5" s="85"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="7"/>
       <c r="K5" s="10" t="s">
         <v>74</v>
@@ -5431,7 +5454,7 @@
       <c r="L5" s="6">
         <v>4</v>
       </c>
-      <c r="M5" s="91"/>
+      <c r="M5" s="88"/>
       <c r="N5" s="7"/>
       <c r="P5" s="10" t="s">
         <v>81</v>
@@ -5439,7 +5462,7 @@
       <c r="Q5" s="32">
         <v>4</v>
       </c>
-      <c r="R5" s="97"/>
+      <c r="R5" s="94"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -5457,7 +5480,7 @@
       <c r="G6" s="6">
         <v>5</v>
       </c>
-      <c r="H6" s="85"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="7"/>
       <c r="K6" s="23" t="s">
         <v>74</v>
@@ -5465,7 +5488,7 @@
       <c r="L6" s="24">
         <v>254</v>
       </c>
-      <c r="M6" s="91"/>
+      <c r="M6" s="88"/>
       <c r="N6" s="25" t="s">
         <v>42</v>
       </c>
@@ -5475,14 +5498,14 @@
       <c r="Q6" s="59">
         <v>254</v>
       </c>
-      <c r="R6" s="97"/>
+      <c r="R6" s="94"/>
       <c r="S6" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="AA6" s="82" t="s">
+      <c r="AA6" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="83"/>
+      <c r="AB6" s="80"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -5499,7 +5522,7 @@
       <c r="G7" s="6">
         <v>6</v>
       </c>
-      <c r="H7" s="85"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="7"/>
       <c r="K7" s="9" t="s">
         <v>74</v>
@@ -5507,7 +5530,7 @@
       <c r="L7" s="3">
         <v>255</v>
       </c>
-      <c r="M7" s="91"/>
+      <c r="M7" s="88"/>
       <c r="N7" s="4" t="s">
         <v>19</v>
       </c>
@@ -5517,7 +5540,7 @@
       <c r="Q7" s="33">
         <v>255</v>
       </c>
-      <c r="R7" s="98"/>
+      <c r="R7" s="95"/>
       <c r="S7" s="4" t="s">
         <v>19</v>
       </c>
@@ -5543,7 +5566,7 @@
       <c r="G8" s="6">
         <v>7</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="82"/>
       <c r="I8" s="7"/>
       <c r="K8" s="9" t="s">
         <v>75</v>
@@ -5551,7 +5574,7 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="91"/>
+      <c r="M8" s="88"/>
       <c r="N8" s="4" t="s">
         <v>23</v>
       </c>
@@ -5577,7 +5600,7 @@
       <c r="G9" s="6">
         <v>8</v>
       </c>
-      <c r="H9" s="85"/>
+      <c r="H9" s="82"/>
       <c r="I9" s="7"/>
       <c r="K9" s="10" t="s">
         <v>75</v>
@@ -5585,7 +5608,7 @@
       <c r="L9" s="6">
         <v>1</v>
       </c>
-      <c r="M9" s="91"/>
+      <c r="M9" s="88"/>
       <c r="N9" s="7"/>
       <c r="P9" s="53" t="s">
         <v>101</v>
@@ -5593,7 +5616,7 @@
       <c r="Q9" s="33">
         <v>0</v>
       </c>
-      <c r="R9" s="92" t="s">
+      <c r="R9" s="89" t="s">
         <v>20</v>
       </c>
       <c r="S9" s="4" t="s">
@@ -5621,7 +5644,7 @@
       <c r="G10" s="6">
         <v>9</v>
       </c>
-      <c r="H10" s="85"/>
+      <c r="H10" s="82"/>
       <c r="I10" s="7"/>
       <c r="K10" s="10" t="s">
         <v>75</v>
@@ -5629,7 +5652,7 @@
       <c r="L10" s="6">
         <v>2</v>
       </c>
-      <c r="M10" s="91"/>
+      <c r="M10" s="88"/>
       <c r="N10" s="7"/>
       <c r="P10" s="54" t="s">
         <v>101</v>
@@ -5637,7 +5660,7 @@
       <c r="Q10" s="32">
         <v>1</v>
       </c>
-      <c r="R10" s="92"/>
+      <c r="R10" s="89"/>
       <c r="S10" s="7" t="s">
         <v>21</v>
       </c>
@@ -5663,7 +5686,7 @@
       <c r="G11" s="6">
         <v>10</v>
       </c>
-      <c r="H11" s="85"/>
+      <c r="H11" s="82"/>
       <c r="I11" s="7"/>
       <c r="K11" s="10" t="s">
         <v>75</v>
@@ -5671,7 +5694,7 @@
       <c r="L11" s="6">
         <v>3</v>
       </c>
-      <c r="M11" s="91"/>
+      <c r="M11" s="88"/>
       <c r="N11" s="7"/>
       <c r="P11" s="54" t="s">
         <v>101</v>
@@ -5679,7 +5702,7 @@
       <c r="Q11" s="32">
         <v>2</v>
       </c>
-      <c r="R11" s="92"/>
+      <c r="R11" s="89"/>
       <c r="S11" s="7" t="s">
         <v>22</v>
       </c>
@@ -5699,7 +5722,7 @@
       <c r="G12" s="6">
         <v>11</v>
       </c>
-      <c r="H12" s="85"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="7"/>
       <c r="K12" s="10" t="s">
         <v>75</v>
@@ -5707,7 +5730,7 @@
       <c r="L12" s="6">
         <v>4</v>
       </c>
-      <c r="M12" s="91"/>
+      <c r="M12" s="88"/>
       <c r="N12" s="7"/>
       <c r="P12" s="69" t="s">
         <v>101</v>
@@ -5715,7 +5738,7 @@
       <c r="Q12" s="34">
         <v>254</v>
       </c>
-      <c r="R12" s="92"/>
+      <c r="R12" s="89"/>
       <c r="S12" s="28" t="s">
         <v>42</v>
       </c>
@@ -5739,7 +5762,7 @@
       <c r="G13" s="6">
         <v>12</v>
       </c>
-      <c r="H13" s="85"/>
+      <c r="H13" s="82"/>
       <c r="I13" s="7"/>
       <c r="K13" s="23" t="s">
         <v>75</v>
@@ -5747,7 +5770,7 @@
       <c r="L13" s="24">
         <v>254</v>
       </c>
-      <c r="M13" s="91"/>
+      <c r="M13" s="88"/>
       <c r="N13" s="25" t="s">
         <v>42</v>
       </c>
@@ -5757,7 +5780,7 @@
       <c r="Q13" s="33">
         <v>255</v>
       </c>
-      <c r="R13" s="92"/>
+      <c r="R13" s="89"/>
       <c r="S13" s="4" t="s">
         <v>19</v>
       </c>
@@ -5781,7 +5804,7 @@
       <c r="G14" s="6">
         <v>13</v>
       </c>
-      <c r="H14" s="85"/>
+      <c r="H14" s="82"/>
       <c r="I14" s="7"/>
       <c r="K14" s="9" t="s">
         <v>75</v>
@@ -5789,7 +5812,7 @@
       <c r="L14" s="3">
         <v>255</v>
       </c>
-      <c r="M14" s="91"/>
+      <c r="M14" s="88"/>
       <c r="N14" s="4" t="s">
         <v>19</v>
       </c>
@@ -5813,7 +5836,7 @@
       <c r="G15" s="6">
         <v>14</v>
       </c>
-      <c r="H15" s="85"/>
+      <c r="H15" s="82"/>
       <c r="I15" s="7"/>
       <c r="K15" s="9" t="s">
         <v>76</v>
@@ -5821,7 +5844,7 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M15" s="91"/>
+      <c r="M15" s="88"/>
       <c r="N15" s="4" t="s">
         <v>23</v>
       </c>
@@ -5831,15 +5854,13 @@
       <c r="Q15" s="58">
         <v>0</v>
       </c>
-      <c r="R15" s="75" t="s">
+      <c r="R15" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="S15" s="57" t="s">
+      <c r="S15" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="T15" s="61" t="s">
-        <v>1</v>
-      </c>
+      <c r="T15" s="125"/>
       <c r="AA15" s="38"/>
       <c r="AB15" s="38"/>
       <c r="AC15" s="38"/>
@@ -5860,7 +5881,7 @@
       <c r="G16" s="6">
         <v>15</v>
       </c>
-      <c r="H16" s="85"/>
+      <c r="H16" s="82"/>
       <c r="I16" s="7"/>
       <c r="K16" s="10" t="s">
         <v>76</v>
@@ -5868,7 +5889,7 @@
       <c r="L16" s="6">
         <v>1</v>
       </c>
-      <c r="M16" s="91"/>
+      <c r="M16" s="88"/>
       <c r="N16" s="7"/>
       <c r="P16" s="32" t="s">
         <v>62</v>
@@ -5876,11 +5897,11 @@
       <c r="Q16" s="32">
         <v>1</v>
       </c>
-      <c r="R16" s="75"/>
-      <c r="S16" s="32" t="s">
+      <c r="R16" s="112"/>
+      <c r="S16" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="T16" s="62"/>
+      <c r="T16" s="125"/>
       <c r="AA16" s="38"/>
       <c r="AB16" s="38"/>
       <c r="AC16" s="38"/>
@@ -5900,7 +5921,7 @@
       <c r="G17" s="6">
         <v>16</v>
       </c>
-      <c r="H17" s="85"/>
+      <c r="H17" s="82"/>
       <c r="I17" s="7"/>
       <c r="K17" s="10" t="s">
         <v>76</v>
@@ -5908,7 +5929,7 @@
       <c r="L17" s="6">
         <v>2</v>
       </c>
-      <c r="M17" s="91"/>
+      <c r="M17" s="88"/>
       <c r="N17" s="7"/>
       <c r="P17" s="32" t="s">
         <v>62</v>
@@ -5916,11 +5937,11 @@
       <c r="Q17" s="32">
         <v>2</v>
       </c>
-      <c r="R17" s="75"/>
-      <c r="S17" s="32" t="s">
+      <c r="R17" s="112"/>
+      <c r="S17" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="T17" s="62"/>
+      <c r="T17" s="125"/>
       <c r="AA17" s="36"/>
       <c r="AB17" s="37"/>
       <c r="AC17" s="37"/>
@@ -5940,7 +5961,7 @@
       <c r="G18" s="6">
         <v>17</v>
       </c>
-      <c r="H18" s="85"/>
+      <c r="H18" s="82"/>
       <c r="I18" s="7"/>
       <c r="K18" s="10" t="s">
         <v>76</v>
@@ -5948,7 +5969,7 @@
       <c r="L18" s="6">
         <v>3</v>
       </c>
-      <c r="M18" s="91"/>
+      <c r="M18" s="88"/>
       <c r="N18" s="7"/>
       <c r="P18" s="32" t="s">
         <v>62</v>
@@ -5956,11 +5977,11 @@
       <c r="Q18" s="32">
         <v>3</v>
       </c>
-      <c r="R18" s="75"/>
-      <c r="S18" s="32" t="s">
+      <c r="R18" s="112"/>
+      <c r="S18" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="T18" s="62"/>
+      <c r="T18" s="125"/>
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
       <c r="AC18" s="22"/>
@@ -5981,7 +6002,7 @@
       <c r="G19" s="6">
         <v>18</v>
       </c>
-      <c r="H19" s="85"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="7"/>
       <c r="K19" s="10" t="s">
         <v>76</v>
@@ -5989,7 +6010,7 @@
       <c r="L19" s="6">
         <v>4</v>
       </c>
-      <c r="M19" s="91"/>
+      <c r="M19" s="88"/>
       <c r="N19" s="7"/>
       <c r="P19" s="32" t="s">
         <v>62</v>
@@ -5997,9 +6018,9 @@
       <c r="Q19" s="32">
         <v>4</v>
       </c>
-      <c r="R19" s="75"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="62"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="125"/>
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
       <c r="AC19" s="22"/>
@@ -6020,7 +6041,7 @@
       <c r="G20" s="6">
         <v>19</v>
       </c>
-      <c r="H20" s="85"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="7"/>
       <c r="K20" s="23" t="s">
         <v>76</v>
@@ -6028,7 +6049,7 @@
       <c r="L20" s="24">
         <v>254</v>
       </c>
-      <c r="M20" s="91"/>
+      <c r="M20" s="88"/>
       <c r="N20" s="25" t="s">
         <v>42</v>
       </c>
@@ -6038,9 +6059,9 @@
       <c r="Q20" s="32">
         <v>5</v>
       </c>
-      <c r="R20" s="75"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="62"/>
+      <c r="R20" s="112"/>
+      <c r="S20" s="121"/>
+      <c r="T20" s="125"/>
       <c r="AA20" s="22"/>
       <c r="AB20" s="22"/>
       <c r="AC20" s="22"/>
@@ -6061,7 +6082,7 @@
       <c r="G21" s="6">
         <v>20</v>
       </c>
-      <c r="H21" s="85"/>
+      <c r="H21" s="82"/>
       <c r="I21" s="7"/>
       <c r="K21" s="9" t="s">
         <v>76</v>
@@ -6069,7 +6090,7 @@
       <c r="L21" s="3">
         <v>255</v>
       </c>
-      <c r="M21" s="91"/>
+      <c r="M21" s="88"/>
       <c r="N21" s="4" t="s">
         <v>19</v>
       </c>
@@ -6079,8 +6100,9 @@
       <c r="Q21" s="32">
         <v>6</v>
       </c>
-      <c r="R21" s="75"/>
-      <c r="T21" s="62"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="121"/>
+      <c r="T21" s="125"/>
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
       <c r="AC21" s="22"/>
@@ -6101,19 +6123,17 @@
       <c r="G22" s="6">
         <v>21</v>
       </c>
-      <c r="H22" s="85"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="7"/>
-      <c r="P22" s="58" t="s">
+      <c r="P22" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Q22" s="58">
+      <c r="Q22" s="32">
         <v>7</v>
       </c>
-      <c r="R22" s="75"/>
-      <c r="S22" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T22" s="63"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="121"/>
+      <c r="T22" s="125"/>
       <c r="AA22" s="22"/>
       <c r="AB22" s="22"/>
       <c r="AC22" s="22"/>
@@ -6134,7 +6154,7 @@
       <c r="G23" s="6">
         <v>22</v>
       </c>
-      <c r="H23" s="85"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="7"/>
       <c r="K23" s="9" t="s">
         <v>77</v>
@@ -6142,25 +6162,21 @@
       <c r="L23" s="3">
         <v>0</v>
       </c>
-      <c r="M23" s="81" t="s">
+      <c r="M23" s="78" t="s">
         <v>16</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="58" t="s">
+      <c r="P23" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Q23" s="58">
+      <c r="Q23" s="32">
         <v>8</v>
       </c>
-      <c r="R23" s="75"/>
-      <c r="S23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="T23" s="61" t="s">
-        <v>0</v>
-      </c>
+      <c r="R23" s="112"/>
+      <c r="S23" s="121"/>
+      <c r="T23" s="125"/>
       <c r="AC23" s="22"/>
       <c r="AD23" s="22"/>
     </row>
@@ -6179,7 +6195,7 @@
       <c r="G24" s="6">
         <v>23</v>
       </c>
-      <c r="H24" s="85"/>
+      <c r="H24" s="82"/>
       <c r="I24" s="7"/>
       <c r="K24" s="10" t="s">
         <v>77</v>
@@ -6187,7 +6203,7 @@
       <c r="L24" s="6">
         <v>1</v>
       </c>
-      <c r="M24" s="81"/>
+      <c r="M24" s="78"/>
       <c r="N24" s="7"/>
       <c r="P24" s="32" t="s">
         <v>62</v>
@@ -6195,11 +6211,11 @@
       <c r="Q24" s="32">
         <v>9</v>
       </c>
-      <c r="R24" s="75"/>
-      <c r="S24" s="32" t="s">
+      <c r="R24" s="112"/>
+      <c r="S24" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="T24" s="62"/>
+      <c r="T24" s="125"/>
       <c r="AC24" s="22"/>
       <c r="AD24" s="22"/>
     </row>
@@ -6218,7 +6234,7 @@
       <c r="G25" s="6">
         <v>24</v>
       </c>
-      <c r="H25" s="85"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="7"/>
       <c r="K25" s="10" t="s">
         <v>77</v>
@@ -6226,7 +6242,7 @@
       <c r="L25" s="6">
         <v>2</v>
       </c>
-      <c r="M25" s="81"/>
+      <c r="M25" s="78"/>
       <c r="N25" s="7"/>
       <c r="P25" s="32" t="s">
         <v>62</v>
@@ -6234,11 +6250,11 @@
       <c r="Q25" s="32">
         <v>10</v>
       </c>
-      <c r="R25" s="75"/>
-      <c r="S25" s="32" t="s">
+      <c r="R25" s="112"/>
+      <c r="S25" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="T25" s="62"/>
+      <c r="T25" s="125"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -6255,7 +6271,7 @@
       <c r="G26" s="6">
         <v>25</v>
       </c>
-      <c r="H26" s="85"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="7"/>
       <c r="K26" s="10" t="s">
         <v>77</v>
@@ -6263,19 +6279,17 @@
       <c r="L26" s="6">
         <v>3</v>
       </c>
-      <c r="M26" s="81"/>
+      <c r="M26" s="78"/>
       <c r="N26" s="7"/>
-      <c r="P26" s="58" t="s">
+      <c r="P26" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Q26" s="58">
+      <c r="Q26" s="32">
         <v>11</v>
       </c>
-      <c r="R26" s="75"/>
-      <c r="S26" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T26" s="62"/>
+      <c r="R26" s="112"/>
+      <c r="S26" s="121"/>
+      <c r="T26" s="125"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -6292,7 +6306,7 @@
       <c r="G27" s="6">
         <v>26</v>
       </c>
-      <c r="H27" s="85"/>
+      <c r="H27" s="82"/>
       <c r="I27" s="7"/>
       <c r="K27" s="10" t="s">
         <v>77</v>
@@ -6300,21 +6314,17 @@
       <c r="L27" s="6">
         <v>4</v>
       </c>
-      <c r="M27" s="81"/>
+      <c r="M27" s="78"/>
       <c r="N27" s="7"/>
-      <c r="P27" s="58" t="s">
+      <c r="P27" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="Q27" s="58">
+      <c r="Q27" s="32">
         <v>12</v>
       </c>
-      <c r="R27" s="75"/>
-      <c r="S27" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="T27" s="61" t="s">
-        <v>0</v>
-      </c>
+      <c r="R27" s="112"/>
+      <c r="S27" s="121"/>
+      <c r="T27" s="125"/>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -6331,7 +6341,7 @@
       <c r="G28" s="6">
         <v>27</v>
       </c>
-      <c r="H28" s="85"/>
+      <c r="H28" s="82"/>
       <c r="I28" s="7"/>
       <c r="K28" s="10" t="s">
         <v>77</v>
@@ -6339,7 +6349,7 @@
       <c r="L28" s="6">
         <v>5</v>
       </c>
-      <c r="M28" s="81"/>
+      <c r="M28" s="78"/>
       <c r="N28" s="7"/>
       <c r="P28" s="32" t="s">
         <v>62</v>
@@ -6347,11 +6357,11 @@
       <c r="Q28" s="32">
         <v>13</v>
       </c>
-      <c r="R28" s="75"/>
-      <c r="S28" s="32" t="s">
+      <c r="R28" s="112"/>
+      <c r="S28" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="T28" s="62"/>
+      <c r="T28" s="125"/>
     </row>
     <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -6368,7 +6378,7 @@
       <c r="G29" s="6">
         <v>28</v>
       </c>
-      <c r="H29" s="85"/>
+      <c r="H29" s="82"/>
       <c r="I29" s="7"/>
       <c r="K29" s="26" t="s">
         <v>77</v>
@@ -6376,7 +6386,7 @@
       <c r="L29" s="27">
         <v>254</v>
       </c>
-      <c r="M29" s="81"/>
+      <c r="M29" s="78"/>
       <c r="N29" s="28" t="s">
         <v>42</v>
       </c>
@@ -6386,11 +6396,11 @@
       <c r="Q29" s="32">
         <v>14</v>
       </c>
-      <c r="R29" s="75"/>
+      <c r="R29" s="112"/>
       <c r="S29" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="T29" s="62"/>
+      <c r="T29" s="125"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -6407,7 +6417,7 @@
       <c r="G30" s="6">
         <v>29</v>
       </c>
-      <c r="H30" s="85"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="7"/>
       <c r="K30" s="9" t="s">
         <v>77</v>
@@ -6415,21 +6425,21 @@
       <c r="L30" s="3">
         <v>255</v>
       </c>
-      <c r="M30" s="81"/>
+      <c r="M30" s="78"/>
       <c r="N30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P30" s="58" t="s">
+      <c r="P30" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="Q30" s="58">
-        <v>15</v>
-      </c>
-      <c r="R30" s="75"/>
-      <c r="S30" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T30" s="63"/>
+      <c r="Q30" s="34">
+        <v>254</v>
+      </c>
+      <c r="R30" s="112"/>
+      <c r="S30" s="126" t="s">
+        <v>124</v>
+      </c>
+      <c r="T30" s="125"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -6446,18 +6456,19 @@
       <c r="G31" s="6">
         <v>30</v>
       </c>
-      <c r="H31" s="85"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="7"/>
       <c r="P31" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q31" s="33">
-        <v>0</v>
-      </c>
-      <c r="R31" s="75"/>
+        <v>255</v>
+      </c>
+      <c r="R31" s="112"/>
       <c r="S31" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="T31" s="125"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
@@ -6474,7 +6485,7 @@
       <c r="G32" s="24">
         <v>254</v>
       </c>
-      <c r="H32" s="85"/>
+      <c r="H32" s="82"/>
       <c r="I32" s="25" t="s">
         <v>91</v>
       </c>
@@ -6484,23 +6495,22 @@
       <c r="L32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="93" t="s">
+      <c r="M32" s="90" t="s">
         <v>24</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P32" s="32" t="s">
+      <c r="P32" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Q32" s="32">
-        <v>1</v>
-      </c>
-      <c r="R32" s="75"/>
-      <c r="S32" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="T32" s="65"/>
+      <c r="Q32" s="33">
+        <v>0</v>
+      </c>
+      <c r="R32" s="112"/>
+      <c r="S32" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -6517,7 +6527,7 @@
       <c r="G33" s="3">
         <v>255</v>
       </c>
-      <c r="H33" s="86"/>
+      <c r="H33" s="83"/>
       <c r="I33" s="4" t="s">
         <v>19</v>
       </c>
@@ -6527,18 +6537,19 @@
       <c r="L33" s="6">
         <v>1</v>
       </c>
-      <c r="M33" s="94"/>
+      <c r="M33" s="91"/>
       <c r="N33" s="7"/>
       <c r="P33" s="32" t="s">
         <v>63</v>
       </c>
       <c r="Q33" s="32">
-        <v>2</v>
-      </c>
-      <c r="R33" s="75"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="112"/>
       <c r="S33" s="32" t="s">
-        <v>52</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="T33" s="65"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
@@ -6555,16 +6566,18 @@
       <c r="L34" s="6">
         <v>2</v>
       </c>
-      <c r="M34" s="94"/>
+      <c r="M34" s="91"/>
       <c r="N34" s="7"/>
       <c r="P34" s="32" t="s">
         <v>63</v>
       </c>
       <c r="Q34" s="32">
-        <v>3</v>
-      </c>
-      <c r="R34" s="75"/>
-      <c r="S34" s="32"/>
+        <v>2</v>
+      </c>
+      <c r="R34" s="112"/>
+      <c r="S34" s="32" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
@@ -6581,7 +6594,7 @@
       <c r="G35" s="3">
         <v>0</v>
       </c>
-      <c r="H35" s="87" t="s">
+      <c r="H35" s="84" t="s">
         <v>15</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -6593,20 +6606,18 @@
       <c r="L35" s="27">
         <v>254</v>
       </c>
-      <c r="M35" s="94"/>
+      <c r="M35" s="91"/>
       <c r="N35" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P35" s="34" t="s">
+      <c r="P35" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="Q35" s="34">
-        <v>4</v>
-      </c>
-      <c r="R35" s="75"/>
-      <c r="S35" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="Q35" s="32">
+        <v>3</v>
+      </c>
+      <c r="R35" s="112"/>
+      <c r="S35" s="32"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
@@ -6623,7 +6634,7 @@
       <c r="G36" s="6">
         <v>1</v>
       </c>
-      <c r="H36" s="88"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="7"/>
       <c r="K36" s="9" t="s">
         <v>78</v>
@@ -6631,19 +6642,19 @@
       <c r="L36" s="3">
         <v>255</v>
       </c>
-      <c r="M36" s="94"/>
+      <c r="M36" s="91"/>
       <c r="N36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P36" s="33" t="s">
+      <c r="P36" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="Q36" s="33">
-        <v>5</v>
-      </c>
-      <c r="R36" s="75"/>
-      <c r="S36" s="4" t="s">
-        <v>19</v>
+      <c r="Q36" s="34">
+        <v>4</v>
+      </c>
+      <c r="R36" s="112"/>
+      <c r="S36" s="28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -6661,7 +6672,7 @@
       <c r="G37" s="6">
         <v>2</v>
       </c>
-      <c r="H37" s="88"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="7"/>
       <c r="K37" s="9" t="s">
         <v>79</v>
@@ -6669,22 +6680,19 @@
       <c r="L37" s="3">
         <v>0</v>
       </c>
-      <c r="M37" s="94"/>
+      <c r="M37" s="91"/>
       <c r="N37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P37" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q37" s="58">
-        <v>0</v>
-      </c>
-      <c r="R37" s="75"/>
-      <c r="S37" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="T37" s="61" t="s">
-        <v>0</v>
+      <c r="P37" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q37" s="33">
+        <v>5</v>
+      </c>
+      <c r="R37" s="112"/>
+      <c r="S37" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -6702,7 +6710,7 @@
       <c r="G38" s="6">
         <v>3</v>
       </c>
-      <c r="H38" s="88"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="7"/>
       <c r="K38" s="10" t="s">
         <v>79</v>
@@ -6710,19 +6718,19 @@
       <c r="L38" s="6">
         <v>1</v>
       </c>
-      <c r="M38" s="94"/>
+      <c r="M38" s="91"/>
       <c r="N38" s="7"/>
-      <c r="P38" s="32" t="s">
+      <c r="P38" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="Q38" s="32">
-        <v>1</v>
-      </c>
-      <c r="R38" s="75"/>
-      <c r="S38" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="T38" s="62"/>
+      <c r="Q38" s="58">
+        <v>0</v>
+      </c>
+      <c r="R38" s="112"/>
+      <c r="S38" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="T38" s="65"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
@@ -6739,7 +6747,7 @@
       <c r="G39" s="6">
         <v>4</v>
       </c>
-      <c r="H39" s="88"/>
+      <c r="H39" s="85"/>
       <c r="I39" s="7"/>
       <c r="K39" s="10" t="s">
         <v>79</v>
@@ -6747,19 +6755,19 @@
       <c r="L39" s="6">
         <v>2</v>
       </c>
-      <c r="M39" s="94"/>
+      <c r="M39" s="91"/>
       <c r="N39" s="7"/>
       <c r="P39" s="32" t="s">
         <v>67</v>
       </c>
       <c r="Q39" s="32">
-        <v>2</v>
-      </c>
-      <c r="R39" s="75"/>
-      <c r="S39" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="T39" s="62"/>
+        <v>1</v>
+      </c>
+      <c r="R39" s="112"/>
+      <c r="S39" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="T39" s="65"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
@@ -6776,7 +6784,7 @@
       <c r="G40" s="6">
         <v>5</v>
       </c>
-      <c r="H40" s="88"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="7"/>
       <c r="K40" s="26" t="s">
         <v>79</v>
@@ -6784,21 +6792,21 @@
       <c r="L40" s="27">
         <v>254</v>
       </c>
-      <c r="M40" s="94"/>
+      <c r="M40" s="91"/>
       <c r="N40" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P40" s="58" t="s">
+      <c r="P40" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="Q40" s="58">
-        <v>3</v>
-      </c>
-      <c r="R40" s="75"/>
-      <c r="S40" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T40" s="62"/>
+      <c r="Q40" s="32">
+        <v>2</v>
+      </c>
+      <c r="R40" s="112"/>
+      <c r="S40" s="120" t="s">
+        <v>47</v>
+      </c>
+      <c r="T40" s="65"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
@@ -6815,7 +6823,7 @@
       <c r="G41" s="6">
         <v>6</v>
       </c>
-      <c r="H41" s="88"/>
+      <c r="H41" s="85"/>
       <c r="I41" s="7"/>
       <c r="K41" s="9" t="s">
         <v>79</v>
@@ -6823,23 +6831,19 @@
       <c r="L41" s="3">
         <v>255</v>
       </c>
-      <c r="M41" s="94"/>
+      <c r="M41" s="91"/>
       <c r="N41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P41" s="58" t="s">
+      <c r="P41" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="Q41" s="58">
-        <v>4</v>
-      </c>
-      <c r="R41" s="75"/>
-      <c r="S41" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="T41" s="61" t="s">
-        <v>0</v>
-      </c>
+      <c r="Q41" s="119">
+        <v>3</v>
+      </c>
+      <c r="R41" s="112"/>
+      <c r="S41" s="121"/>
+      <c r="T41" s="65"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
@@ -6856,7 +6860,7 @@
       <c r="G42" s="6">
         <v>7</v>
       </c>
-      <c r="H42" s="88"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="7"/>
       <c r="K42" s="9" t="s">
         <v>80</v>
@@ -6864,21 +6868,19 @@
       <c r="L42" s="3">
         <v>0</v>
       </c>
-      <c r="M42" s="94"/>
+      <c r="M42" s="91"/>
       <c r="N42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P42" s="32" t="s">
+      <c r="P42" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="Q42" s="32">
-        <v>5</v>
-      </c>
-      <c r="R42" s="75"/>
-      <c r="S42" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="T42" s="62"/>
+      <c r="Q42" s="119">
+        <v>4</v>
+      </c>
+      <c r="R42" s="112"/>
+      <c r="S42" s="121"/>
+      <c r="T42" s="65"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
@@ -6895,7 +6897,7 @@
       <c r="G43" s="6">
         <v>8</v>
       </c>
-      <c r="H43" s="88"/>
+      <c r="H43" s="85"/>
       <c r="I43" s="7"/>
       <c r="K43" s="10" t="s">
         <v>80</v>
@@ -6903,19 +6905,19 @@
       <c r="L43" s="6">
         <v>1</v>
       </c>
-      <c r="M43" s="94"/>
+      <c r="M43" s="91"/>
       <c r="N43" s="7"/>
       <c r="P43" s="32" t="s">
         <v>67</v>
       </c>
       <c r="Q43" s="32">
-        <v>6</v>
-      </c>
-      <c r="R43" s="75"/>
-      <c r="S43" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="T43" s="62"/>
+        <v>5</v>
+      </c>
+      <c r="R43" s="112"/>
+      <c r="S43" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="T43" s="65"/>
     </row>
     <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
@@ -6932,7 +6934,7 @@
       <c r="G44" s="6">
         <v>9</v>
       </c>
-      <c r="H44" s="88"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="7"/>
       <c r="K44" s="10" t="s">
         <v>80</v>
@@ -6940,19 +6942,19 @@
       <c r="L44" s="6">
         <v>2</v>
       </c>
-      <c r="M44" s="94"/>
+      <c r="M44" s="91"/>
       <c r="N44" s="7"/>
-      <c r="P44" s="58" t="s">
+      <c r="P44" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="Q44" s="58">
-        <v>7</v>
-      </c>
-      <c r="R44" s="75"/>
-      <c r="S44" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T44" s="63"/>
+      <c r="Q44" s="32">
+        <v>6</v>
+      </c>
+      <c r="R44" s="112"/>
+      <c r="S44" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="T44" s="65"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
@@ -6969,7 +6971,7 @@
       <c r="G45" s="6">
         <v>10</v>
       </c>
-      <c r="H45" s="88"/>
+      <c r="H45" s="85"/>
       <c r="I45" s="7"/>
       <c r="K45" s="26" t="s">
         <v>80</v>
@@ -6977,23 +6979,19 @@
       <c r="L45" s="27">
         <v>254</v>
       </c>
-      <c r="M45" s="94"/>
+      <c r="M45" s="91"/>
       <c r="N45" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P45" s="58" t="s">
+      <c r="P45" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="Q45" s="58">
-        <v>8</v>
-      </c>
-      <c r="R45" s="75"/>
-      <c r="S45" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="T45" s="62" t="s">
-        <v>0</v>
-      </c>
+      <c r="Q45" s="119">
+        <v>7</v>
+      </c>
+      <c r="R45" s="112"/>
+      <c r="S45" s="121"/>
+      <c r="T45" s="65"/>
     </row>
     <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
@@ -7010,7 +7008,7 @@
       <c r="G46" s="24">
         <v>254</v>
       </c>
-      <c r="H46" s="88"/>
+      <c r="H46" s="85"/>
       <c r="I46" s="25" t="s">
         <v>92</v>
       </c>
@@ -7020,21 +7018,19 @@
       <c r="L46" s="3">
         <v>255</v>
       </c>
-      <c r="M46" s="95"/>
+      <c r="M46" s="92"/>
       <c r="N46" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P46" s="32" t="s">
+      <c r="P46" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="Q46" s="32">
-        <v>9</v>
-      </c>
-      <c r="R46" s="75"/>
-      <c r="S46" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="T46" s="62"/>
+      <c r="Q46" s="119">
+        <v>8</v>
+      </c>
+      <c r="R46" s="112"/>
+      <c r="S46" s="121"/>
+      <c r="T46" s="65"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
@@ -7051,7 +7047,7 @@
       <c r="G47" s="3">
         <v>255</v>
       </c>
-      <c r="H47" s="89"/>
+      <c r="H47" s="86"/>
       <c r="I47" s="4" t="s">
         <v>19</v>
       </c>
@@ -7059,13 +7055,13 @@
         <v>67</v>
       </c>
       <c r="Q47" s="32">
-        <v>10</v>
-      </c>
-      <c r="R47" s="75"/>
-      <c r="S47" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="T47" s="62"/>
+        <v>9</v>
+      </c>
+      <c r="R47" s="112"/>
+      <c r="S47" s="120" t="s">
+        <v>55</v>
+      </c>
+      <c r="T47" s="65"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -7076,17 +7072,17 @@
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="7"/>
-      <c r="P48" s="58" t="s">
+      <c r="P48" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="Q48" s="58">
-        <v>11</v>
-      </c>
-      <c r="R48" s="75"/>
-      <c r="S48" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="T48" s="63"/>
+      <c r="Q48" s="32">
+        <v>10</v>
+      </c>
+      <c r="R48" s="112"/>
+      <c r="S48" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="T48" s="65"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -7097,16 +7093,17 @@
       </c>
       <c r="C49" s="73"/>
       <c r="D49" s="7"/>
-      <c r="P49" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q49" s="33">
-        <v>0</v>
-      </c>
-      <c r="R49" s="75"/>
-      <c r="S49" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="P49" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q49" s="34">
+        <v>254</v>
+      </c>
+      <c r="R49" s="112"/>
+      <c r="S49" s="126" t="s">
+        <v>123</v>
+      </c>
+      <c r="T49" s="65"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
@@ -7117,17 +7114,17 @@
       </c>
       <c r="C50" s="73"/>
       <c r="D50" s="7"/>
-      <c r="P50" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q50" s="32">
-        <v>1</v>
-      </c>
-      <c r="R50" s="75"/>
-      <c r="S50" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="T50" s="65"/>
+      <c r="P50" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q50" s="33">
+        <v>255</v>
+      </c>
+      <c r="R50" s="112"/>
+      <c r="S50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T50" s="125"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
@@ -7138,16 +7135,6 @@
       </c>
       <c r="C51" s="73"/>
       <c r="D51" s="7"/>
-      <c r="P51" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q51" s="32">
-        <v>2</v>
-      </c>
-      <c r="R51" s="75"/>
-      <c r="S51" s="32" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
@@ -7160,14 +7147,6 @@
       <c r="D52" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="P52" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q52" s="32">
-        <v>3</v>
-      </c>
-      <c r="R52" s="75"/>
-      <c r="S52" s="32"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
@@ -7180,16 +7159,6 @@
       <c r="D53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P53" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q53" s="34">
-        <v>254</v>
-      </c>
-      <c r="R53" s="75"/>
-      <c r="S53" s="28" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="67" t="s">
@@ -7202,16 +7171,6 @@
       <c r="D54" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="P54" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q54" s="33">
-        <v>255</v>
-      </c>
-      <c r="R54" s="75"/>
-      <c r="S54" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
@@ -7232,21 +7191,6 @@
       </c>
       <c r="C56" s="73"/>
       <c r="D56" s="7"/>
-      <c r="P56" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q56" s="33">
-        <v>0</v>
-      </c>
-      <c r="R56" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="S56" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="T56" s="61" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -7257,19 +7201,8 @@
       </c>
       <c r="C57" s="73"/>
       <c r="D57" s="7"/>
-      <c r="P57" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q57" s="32">
-        <v>1</v>
-      </c>
-      <c r="R57" s="76"/>
-      <c r="S57" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="T57" s="62"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>60</v>
       </c>
@@ -7278,17 +7211,6 @@
       </c>
       <c r="C58" s="73"/>
       <c r="D58" s="7"/>
-      <c r="P58" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q58" s="32">
-        <v>2</v>
-      </c>
-      <c r="R58" s="76"/>
-      <c r="S58" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="T58" s="62"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
@@ -7299,17 +7221,6 @@
       </c>
       <c r="C59" s="73"/>
       <c r="D59" s="7"/>
-      <c r="P59" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q59" s="33">
-        <v>3</v>
-      </c>
-      <c r="R59" s="76"/>
-      <c r="S59" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T59" s="63"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
@@ -7330,21 +7241,6 @@
       </c>
       <c r="C61" s="73"/>
       <c r="D61" s="7"/>
-      <c r="P61" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q61" s="60">
-        <v>1</v>
-      </c>
-      <c r="R61" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="S61" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="T61" s="60" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
@@ -7355,22 +7251,9 @@
       </c>
       <c r="C62" s="73"/>
       <c r="D62" s="7"/>
-      <c r="P62" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q62" s="60">
-        <v>2</v>
-      </c>
-      <c r="R62" s="77"/>
-      <c r="S62" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="T62" s="60" t="s">
-        <v>111</v>
-      </c>
       <c r="W62" s="52"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>60</v>
       </c>
@@ -7379,19 +7262,6 @@
       </c>
       <c r="C63" s="73"/>
       <c r="D63" s="7"/>
-      <c r="P63" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q63" s="60">
-        <v>1</v>
-      </c>
-      <c r="R63" s="77"/>
-      <c r="S63" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="T63" s="60" t="s">
-        <v>111</v>
-      </c>
       <c r="W63" s="52"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -7403,19 +7273,6 @@
       </c>
       <c r="C64" s="73"/>
       <c r="D64" s="7"/>
-      <c r="P64" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q64" s="60">
-        <v>1</v>
-      </c>
-      <c r="R64" s="77"/>
-      <c r="S64" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="T64" s="60" t="s">
-        <v>111</v>
-      </c>
       <c r="W64" s="52"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
@@ -7427,19 +7284,6 @@
       </c>
       <c r="C65" s="73"/>
       <c r="D65" s="7"/>
-      <c r="P65" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q65" s="60">
-        <v>2</v>
-      </c>
-      <c r="R65" s="77"/>
-      <c r="S65" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="T65" s="60" t="s">
-        <v>111</v>
-      </c>
       <c r="W65" s="52"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
@@ -7451,19 +7295,6 @@
       </c>
       <c r="C66" s="73"/>
       <c r="D66" s="7"/>
-      <c r="P66" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q66" s="60">
-        <v>1</v>
-      </c>
-      <c r="R66" s="77"/>
-      <c r="S66" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="T66" s="60" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -7494,6 +7325,16 @@
       </c>
       <c r="C69" s="73"/>
       <c r="D69" s="7"/>
+      <c r="P69" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q69" s="33">
+        <v>0</v>
+      </c>
+      <c r="R69" s="117"/>
+      <c r="S69" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
@@ -7504,6 +7345,17 @@
       </c>
       <c r="C70" s="73"/>
       <c r="D70" s="7"/>
+      <c r="P70" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q70" s="32">
+        <v>1</v>
+      </c>
+      <c r="R70" s="117"/>
+      <c r="S70" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="T70" s="65"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
@@ -7514,6 +7366,16 @@
       </c>
       <c r="C71" s="73"/>
       <c r="D71" s="7"/>
+      <c r="P71" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q71" s="32">
+        <v>2</v>
+      </c>
+      <c r="R71" s="117"/>
+      <c r="S71" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
@@ -7524,6 +7386,14 @@
       </c>
       <c r="C72" s="73"/>
       <c r="D72" s="7"/>
+      <c r="P72" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q72" s="32">
+        <v>3</v>
+      </c>
+      <c r="R72" s="117"/>
+      <c r="S72" s="32"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
@@ -7534,6 +7404,16 @@
       </c>
       <c r="C73" s="73"/>
       <c r="D73" s="7"/>
+      <c r="P73" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q73" s="34">
+        <v>254</v>
+      </c>
+      <c r="R73" s="117"/>
+      <c r="S73" s="28" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
@@ -7544,6 +7424,16 @@
       </c>
       <c r="C74" s="73"/>
       <c r="D74" s="7"/>
+      <c r="P74" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q74" s="33">
+        <v>255</v>
+      </c>
+      <c r="R74" s="118"/>
+      <c r="S74" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
@@ -7564,6 +7454,21 @@
       </c>
       <c r="C76" s="73"/>
       <c r="D76" s="7"/>
+      <c r="P76" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q76" s="33">
+        <v>0</v>
+      </c>
+      <c r="R76" s="114" t="s">
+        <v>118</v>
+      </c>
+      <c r="S76" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T76" s="61" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
@@ -7574,6 +7479,17 @@
       </c>
       <c r="C77" s="73"/>
       <c r="D77" s="7"/>
+      <c r="P77" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q77" s="32">
+        <v>1</v>
+      </c>
+      <c r="R77" s="115"/>
+      <c r="S77" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="T77" s="62"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
@@ -7584,6 +7500,17 @@
       </c>
       <c r="C78" s="73"/>
       <c r="D78" s="7"/>
+      <c r="P78" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q78" s="32">
+        <v>2</v>
+      </c>
+      <c r="R78" s="115"/>
+      <c r="S78" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="T78" s="62"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
@@ -7594,6 +7521,17 @@
       </c>
       <c r="C79" s="73"/>
       <c r="D79" s="7"/>
+      <c r="P79" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q79" s="33">
+        <v>3</v>
+      </c>
+      <c r="R79" s="116"/>
+      <c r="S79" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T79" s="63"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
@@ -7605,7 +7543,7 @@
       <c r="C80" s="73"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>60</v>
       </c>
@@ -7614,8 +7552,23 @@
       </c>
       <c r="C81" s="73"/>
       <c r="D81" s="7"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P81" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q81" s="60">
+        <v>1</v>
+      </c>
+      <c r="R81" s="122" t="s">
+        <v>119</v>
+      </c>
+      <c r="S81" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="T81" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>60</v>
       </c>
@@ -7624,8 +7577,21 @@
       </c>
       <c r="C82" s="73"/>
       <c r="D82" s="7"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P82" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q82" s="60">
+        <v>2</v>
+      </c>
+      <c r="R82" s="123"/>
+      <c r="S82" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="T82" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>60</v>
       </c>
@@ -7634,8 +7600,21 @@
       </c>
       <c r="C83" s="73"/>
       <c r="D83" s="7"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P83" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q83" s="60">
+        <v>1</v>
+      </c>
+      <c r="R83" s="123"/>
+      <c r="S83" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="T83" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>60</v>
       </c>
@@ -7644,8 +7623,21 @@
       </c>
       <c r="C84" s="73"/>
       <c r="D84" s="7"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P84" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q84" s="60">
+        <v>1</v>
+      </c>
+      <c r="R84" s="123"/>
+      <c r="S84" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="T84" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>60</v>
       </c>
@@ -7654,8 +7646,21 @@
       </c>
       <c r="C85" s="73"/>
       <c r="D85" s="7"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P85" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q85" s="60">
+        <v>2</v>
+      </c>
+      <c r="R85" s="123"/>
+      <c r="S85" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="T85" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>60</v>
       </c>
@@ -7664,8 +7669,21 @@
       </c>
       <c r="C86" s="73"/>
       <c r="D86" s="7"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="P86" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q86" s="60">
+        <v>1</v>
+      </c>
+      <c r="R86" s="124"/>
+      <c r="S86" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="T86" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>60</v>
       </c>
@@ -7675,7 +7693,7 @@
       <c r="C87" s="73"/>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>60</v>
       </c>
@@ -7685,7 +7703,7 @@
       <c r="C88" s="73"/>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>60</v>
       </c>
@@ -7695,7 +7713,7 @@
       <c r="C89" s="73"/>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>60</v>
       </c>
@@ -7705,7 +7723,7 @@
       <c r="C90" s="73"/>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>60</v>
       </c>
@@ -7715,7 +7733,7 @@
       <c r="C91" s="73"/>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>60</v>
       </c>
@@ -7725,7 +7743,7 @@
       <c r="C92" s="73"/>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>60</v>
       </c>
@@ -7735,7 +7753,7 @@
       <c r="C93" s="73"/>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>60</v>
       </c>
@@ -7745,7 +7763,7 @@
       <c r="C94" s="73"/>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
         <v>60</v>
       </c>
@@ -7757,7 +7775,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="67" t="s">
         <v>60</v>
       </c>
@@ -8304,9 +8322,8 @@
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="C1:C148"/>
-    <mergeCell ref="R15:R54"/>
-    <mergeCell ref="R56:R59"/>
-    <mergeCell ref="R61:R66"/>
+    <mergeCell ref="R76:R79"/>
+    <mergeCell ref="R81:R86"/>
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="M23:M30"/>
     <mergeCell ref="AA6:AB6"/>
@@ -8316,6 +8333,7 @@
     <mergeCell ref="R9:R13"/>
     <mergeCell ref="M32:M46"/>
     <mergeCell ref="R1:R7"/>
+    <mergeCell ref="R15:R50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -8326,8 +8344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EEFD53-ADB5-4FC2-BDE3-F23A2E6D7C28}">
   <dimension ref="A1:AF144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="AB35" sqref="AB35"/>
+    <sheetView topLeftCell="G21" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8377,7 +8395,7 @@
         <v>38</v>
       </c>
       <c r="G1" s="3"/>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="81" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -8387,7 +8405,7 @@
         <v>85</v>
       </c>
       <c r="L1" s="3"/>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="96" t="s">
         <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -8397,7 +8415,7 @@
         <v>99</v>
       </c>
       <c r="Q1" s="3"/>
-      <c r="R1" s="96" t="s">
+      <c r="R1" s="93" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -8421,7 +8439,7 @@
         <f>DEC2HEX('ipv4'!G2)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="85"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="55"/>
       <c r="K2" s="10" t="s">
         <v>85</v>
@@ -8430,7 +8448,7 @@
         <f>DEC2HEX('ipv4'!L2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="109"/>
+      <c r="M2" s="97"/>
       <c r="N2" s="55"/>
       <c r="P2" s="10" t="s">
         <v>99</v>
@@ -8439,18 +8457,18 @@
         <f>DEC2HEX('ipv4'!Q2)</f>
         <v>1</v>
       </c>
-      <c r="R2" s="97"/>
+      <c r="R2" s="94"/>
       <c r="S2" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="78" t="s">
+      <c r="AA2" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="80"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="76"/>
+      <c r="AF2" s="77"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -8469,7 +8487,7 @@
         <f>DEC2HEX('ipv4'!G3)</f>
         <v>2</v>
       </c>
-      <c r="H3" s="85"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="55"/>
       <c r="K3" s="10" t="s">
         <v>85</v>
@@ -8478,7 +8496,7 @@
         <f>DEC2HEX('ipv4'!L3)</f>
         <v>2</v>
       </c>
-      <c r="M3" s="109"/>
+      <c r="M3" s="97"/>
       <c r="N3" s="55"/>
       <c r="P3" s="10" t="s">
         <v>99</v>
@@ -8487,15 +8505,15 @@
         <f>DEC2HEX('ipv4'!Q3)</f>
         <v>2</v>
       </c>
-      <c r="R3" s="97"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="AA3" s="117" t="s">
+      <c r="AA3" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="119"/>
+      <c r="AB3" s="106"/>
+      <c r="AC3" s="107"/>
       <c r="AD3" s="16" t="s">
         <v>86</v>
       </c>
@@ -8523,7 +8541,7 @@
         <f>DEC2HEX('ipv4'!G4)</f>
         <v>3</v>
       </c>
-      <c r="H4" s="85"/>
+      <c r="H4" s="82"/>
       <c r="I4" s="55"/>
       <c r="K4" s="10" t="s">
         <v>85</v>
@@ -8532,7 +8550,7 @@
         <f>DEC2HEX('ipv4'!L4)</f>
         <v>3</v>
       </c>
-      <c r="M4" s="109"/>
+      <c r="M4" s="97"/>
       <c r="N4" s="55"/>
       <c r="P4" s="10" t="s">
         <v>99</v>
@@ -8541,7 +8559,7 @@
         <f>DEC2HEX('ipv4'!Q4)</f>
         <v>3</v>
       </c>
-      <c r="R4" s="97"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="55"/>
       <c r="AA4" s="41">
         <v>2001</v>
@@ -8579,7 +8597,7 @@
         <f>DEC2HEX('ipv4'!G5)</f>
         <v>4</v>
       </c>
-      <c r="H5" s="85"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="55"/>
       <c r="K5" s="10" t="s">
         <v>85</v>
@@ -8588,7 +8606,7 @@
         <f>DEC2HEX('ipv4'!L5)</f>
         <v>4</v>
       </c>
-      <c r="M5" s="109"/>
+      <c r="M5" s="97"/>
       <c r="N5" s="55"/>
       <c r="P5" s="10" t="s">
         <v>99</v>
@@ -8597,7 +8615,7 @@
         <f>DEC2HEX('ipv4'!Q5)</f>
         <v>4</v>
       </c>
-      <c r="R5" s="98"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="55"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8617,20 +8635,20 @@
         <f>DEC2HEX('ipv4'!G6)</f>
         <v>5</v>
       </c>
-      <c r="H6" s="85"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="55"/>
       <c r="K6" s="9" t="s">
         <v>93</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="109"/>
+      <c r="M6" s="97"/>
       <c r="N6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA6" s="82" t="s">
+      <c r="AA6" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="83"/>
+      <c r="AB6" s="80"/>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -8649,7 +8667,7 @@
         <f>DEC2HEX('ipv4'!G7)</f>
         <v>6</v>
       </c>
-      <c r="H7" s="85"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="55"/>
       <c r="K7" s="10" t="s">
         <v>93</v>
@@ -8658,13 +8676,13 @@
         <f>DEC2HEX('ipv4'!L9)</f>
         <v>1</v>
       </c>
-      <c r="M7" s="109"/>
+      <c r="M7" s="97"/>
       <c r="N7" s="55"/>
       <c r="P7" s="9" t="s">
         <v>100</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="96" t="s">
+      <c r="R7" s="93" t="s">
         <v>20</v>
       </c>
       <c r="S7" s="4" t="s">
@@ -8694,7 +8712,7 @@
         <f>DEC2HEX('ipv4'!G8)</f>
         <v>7</v>
       </c>
-      <c r="H8" s="85"/>
+      <c r="H8" s="82"/>
       <c r="I8" s="55"/>
       <c r="K8" s="10" t="s">
         <v>93</v>
@@ -8703,7 +8721,7 @@
         <f>DEC2HEX('ipv4'!L10)</f>
         <v>2</v>
       </c>
-      <c r="M8" s="109"/>
+      <c r="M8" s="97"/>
       <c r="N8" s="55"/>
       <c r="P8" s="10" t="s">
         <v>100</v>
@@ -8712,7 +8730,7 @@
         <f>DEC2HEX('ipv4'!Q10)</f>
         <v>1</v>
       </c>
-      <c r="R8" s="97"/>
+      <c r="R8" s="94"/>
       <c r="S8" s="55" t="s">
         <v>21</v>
       </c>
@@ -8740,7 +8758,7 @@
         <f>DEC2HEX('ipv4'!G9)</f>
         <v>8</v>
       </c>
-      <c r="H9" s="85"/>
+      <c r="H9" s="82"/>
       <c r="I9" s="55"/>
       <c r="K9" s="10" t="s">
         <v>93</v>
@@ -8749,7 +8767,7 @@
         <f>DEC2HEX('ipv4'!L11)</f>
         <v>3</v>
       </c>
-      <c r="M9" s="109"/>
+      <c r="M9" s="97"/>
       <c r="N9" s="55"/>
       <c r="P9" s="10" t="s">
         <v>100</v>
@@ -8758,7 +8776,7 @@
         <f>DEC2HEX('ipv4'!Q11)</f>
         <v>2</v>
       </c>
-      <c r="R9" s="98"/>
+      <c r="R9" s="95"/>
       <c r="S9" s="55" t="s">
         <v>22</v>
       </c>
@@ -8786,7 +8804,7 @@
         <f>DEC2HEX('ipv4'!G10)</f>
         <v>9</v>
       </c>
-      <c r="H10" s="85"/>
+      <c r="H10" s="82"/>
       <c r="I10" s="55"/>
       <c r="K10" s="10" t="s">
         <v>93</v>
@@ -8795,7 +8813,7 @@
         <f>DEC2HEX('ipv4'!L12)</f>
         <v>4</v>
       </c>
-      <c r="M10" s="109"/>
+      <c r="M10" s="97"/>
       <c r="N10" s="55"/>
       <c r="AA10" s="40" t="s">
         <v>83</v>
@@ -8821,13 +8839,13 @@
         <f>DEC2HEX('ipv4'!G11)</f>
         <v>A</v>
       </c>
-      <c r="H11" s="85"/>
+      <c r="H11" s="82"/>
       <c r="I11" s="55"/>
       <c r="K11" s="9" t="s">
         <v>94</v>
       </c>
       <c r="L11" s="3"/>
-      <c r="M11" s="109"/>
+      <c r="M11" s="97"/>
       <c r="N11" s="4" t="s">
         <v>23</v>
       </c>
@@ -8835,7 +8853,7 @@
         <v>102</v>
       </c>
       <c r="Q11" s="33"/>
-      <c r="R11" s="102" t="s">
+      <c r="R11" s="111" t="s">
         <v>71</v>
       </c>
       <c r="S11" s="4" t="s">
@@ -8859,7 +8877,7 @@
         <f>DEC2HEX('ipv4'!G12)</f>
         <v>B</v>
       </c>
-      <c r="H12" s="85"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="55"/>
       <c r="K12" s="10" t="s">
         <v>94</v>
@@ -8868,7 +8886,7 @@
         <f>DEC2HEX('ipv4'!L16)</f>
         <v>1</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="97"/>
       <c r="N12" s="55"/>
       <c r="P12" s="54" t="s">
         <v>102</v>
@@ -8877,7 +8895,7 @@
         <f>DEC2HEX('ipv4'!Q16)</f>
         <v>1</v>
       </c>
-      <c r="R12" s="103"/>
+      <c r="R12" s="112"/>
       <c r="S12" s="32" t="s">
         <v>56</v>
       </c>
@@ -8903,7 +8921,7 @@
         <f>DEC2HEX('ipv4'!G13)</f>
         <v>C</v>
       </c>
-      <c r="H13" s="85"/>
+      <c r="H13" s="82"/>
       <c r="I13" s="55"/>
       <c r="K13" s="10" t="s">
         <v>94</v>
@@ -8912,7 +8930,7 @@
         <f>DEC2HEX('ipv4'!L17)</f>
         <v>2</v>
       </c>
-      <c r="M13" s="109"/>
+      <c r="M13" s="97"/>
       <c r="N13" s="55"/>
       <c r="P13" s="54" t="s">
         <v>102</v>
@@ -8921,7 +8939,7 @@
         <f>DEC2HEX('ipv4'!Q17)</f>
         <v>2</v>
       </c>
-      <c r="R13" s="103"/>
+      <c r="R13" s="112"/>
       <c r="S13" s="32" t="s">
         <v>57</v>
       </c>
@@ -8947,7 +8965,7 @@
         <f>DEC2HEX('ipv4'!G14)</f>
         <v>D</v>
       </c>
-      <c r="H14" s="85"/>
+      <c r="H14" s="82"/>
       <c r="I14" s="55"/>
       <c r="K14" s="10" t="s">
         <v>94</v>
@@ -8956,7 +8974,7 @@
         <f>DEC2HEX('ipv4'!L18)</f>
         <v>3</v>
       </c>
-      <c r="M14" s="109"/>
+      <c r="M14" s="97"/>
       <c r="N14" s="55"/>
       <c r="P14" s="54" t="s">
         <v>102</v>
@@ -8965,7 +8983,7 @@
         <f>DEC2HEX('ipv4'!Q18)</f>
         <v>3</v>
       </c>
-      <c r="R14" s="103"/>
+      <c r="R14" s="112"/>
       <c r="S14" s="32" t="s">
         <v>58</v>
       </c>
@@ -8991,7 +9009,7 @@
         <f>DEC2HEX('ipv4'!G15)</f>
         <v>E</v>
       </c>
-      <c r="H15" s="85"/>
+      <c r="H15" s="82"/>
       <c r="I15" s="55"/>
       <c r="K15" s="10" t="s">
         <v>94</v>
@@ -9000,7 +9018,7 @@
         <f>DEC2HEX('ipv4'!L19)</f>
         <v>4</v>
       </c>
-      <c r="M15" s="110"/>
+      <c r="M15" s="98"/>
       <c r="N15" s="55"/>
       <c r="P15" s="54" t="s">
         <v>102</v>
@@ -9009,7 +9027,7 @@
         <f>DEC2HEX('ipv4'!Q19)</f>
         <v>4</v>
       </c>
-      <c r="R15" s="103"/>
+      <c r="R15" s="112"/>
       <c r="S15" s="32"/>
       <c r="AA15" s="38"/>
       <c r="AB15" s="38"/>
@@ -9033,7 +9051,7 @@
         <f>DEC2HEX('ipv4'!G16)</f>
         <v>F</v>
       </c>
-      <c r="H16" s="85"/>
+      <c r="H16" s="82"/>
       <c r="I16" s="55"/>
       <c r="M16" s="29"/>
       <c r="P16" s="54" t="s">
@@ -9043,7 +9061,7 @@
         <f>DEC2HEX('ipv4'!Q20)</f>
         <v>5</v>
       </c>
-      <c r="R16" s="103"/>
+      <c r="R16" s="112"/>
       <c r="S16" s="32"/>
       <c r="AA16" s="38"/>
       <c r="AB16" s="38"/>
@@ -9067,13 +9085,13 @@
         <f>DEC2HEX('ipv4'!G17)</f>
         <v>10</v>
       </c>
-      <c r="H17" s="85"/>
+      <c r="H17" s="82"/>
       <c r="I17" s="55"/>
       <c r="K17" s="9" t="s">
         <v>95</v>
       </c>
       <c r="L17" s="3"/>
-      <c r="M17" s="111" t="s">
+      <c r="M17" s="99" t="s">
         <v>16</v>
       </c>
       <c r="N17" s="4" t="s">
@@ -9086,7 +9104,7 @@
         <f>DEC2HEX('ipv4'!Q21)</f>
         <v>6</v>
       </c>
-      <c r="R17" s="103"/>
+      <c r="R17" s="112"/>
       <c r="S17" s="32"/>
       <c r="AA17" s="36"/>
       <c r="AB17" s="22"/>
@@ -9110,7 +9128,7 @@
         <f>DEC2HEX('ipv4'!G18)</f>
         <v>11</v>
       </c>
-      <c r="H18" s="85"/>
+      <c r="H18" s="82"/>
       <c r="I18" s="55"/>
       <c r="K18" s="10" t="s">
         <v>95</v>
@@ -9119,7 +9137,7 @@
         <f>DEC2HEX('ipv4'!L24)</f>
         <v>1</v>
       </c>
-      <c r="M18" s="112"/>
+      <c r="M18" s="100"/>
       <c r="N18" s="55"/>
       <c r="P18" s="54" t="s">
         <v>102</v>
@@ -9128,7 +9146,7 @@
         <f>DEC2HEX('ipv4'!Q23)</f>
         <v>8</v>
       </c>
-      <c r="R18" s="103"/>
+      <c r="R18" s="112"/>
       <c r="S18" s="70"/>
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
@@ -9152,7 +9170,7 @@
         <f>DEC2HEX('ipv4'!G19)</f>
         <v>12</v>
       </c>
-      <c r="H19" s="85"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="55"/>
       <c r="K19" s="10" t="s">
         <v>95</v>
@@ -9161,7 +9179,7 @@
         <f>DEC2HEX('ipv4'!L25)</f>
         <v>2</v>
       </c>
-      <c r="M19" s="112"/>
+      <c r="M19" s="100"/>
       <c r="N19" s="55"/>
       <c r="P19" s="54" t="s">
         <v>102</v>
@@ -9170,7 +9188,7 @@
         <f>DEC2HEX('ipv4'!Q24)</f>
         <v>9</v>
       </c>
-      <c r="R19" s="103"/>
+      <c r="R19" s="112"/>
       <c r="S19" s="32" t="s">
         <v>49</v>
       </c>
@@ -9196,7 +9214,7 @@
         <f>DEC2HEX('ipv4'!G20)</f>
         <v>13</v>
       </c>
-      <c r="H20" s="85"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="55"/>
       <c r="K20" s="10" t="s">
         <v>95</v>
@@ -9205,7 +9223,7 @@
         <f>DEC2HEX('ipv4'!L26)</f>
         <v>3</v>
       </c>
-      <c r="M20" s="112"/>
+      <c r="M20" s="100"/>
       <c r="N20" s="55"/>
       <c r="P20" s="54" t="s">
         <v>102</v>
@@ -9214,7 +9232,7 @@
         <f>DEC2HEX('ipv4'!Q25)</f>
         <v>A</v>
       </c>
-      <c r="R20" s="103"/>
+      <c r="R20" s="112"/>
       <c r="S20" s="32" t="s">
         <v>51</v>
       </c>
@@ -9240,7 +9258,7 @@
         <f>DEC2HEX('ipv4'!G21)</f>
         <v>14</v>
       </c>
-      <c r="H21" s="85"/>
+      <c r="H21" s="82"/>
       <c r="I21" s="55"/>
       <c r="K21" s="10" t="s">
         <v>95</v>
@@ -9249,7 +9267,7 @@
         <f>DEC2HEX('ipv4'!L27)</f>
         <v>4</v>
       </c>
-      <c r="M21" s="112"/>
+      <c r="M21" s="100"/>
       <c r="N21" s="55"/>
       <c r="P21" s="54" t="s">
         <v>102</v>
@@ -9258,7 +9276,7 @@
         <f>DEC2HEX('ipv4'!Q27)</f>
         <v>C</v>
       </c>
-      <c r="R21" s="103"/>
+      <c r="R21" s="112"/>
       <c r="S21" s="70"/>
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
@@ -9282,7 +9300,7 @@
         <f>DEC2HEX('ipv4'!G22)</f>
         <v>15</v>
       </c>
-      <c r="H22" s="85"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="55"/>
       <c r="K22" s="10" t="s">
         <v>95</v>
@@ -9291,7 +9309,7 @@
         <f>DEC2HEX('ipv4'!L28)</f>
         <v>5</v>
       </c>
-      <c r="M22" s="113"/>
+      <c r="M22" s="101"/>
       <c r="N22" s="55"/>
       <c r="P22" s="54" t="s">
         <v>102</v>
@@ -9300,7 +9318,7 @@
         <f>DEC2HEX('ipv4'!Q28)</f>
         <v>D</v>
       </c>
-      <c r="R22" s="103"/>
+      <c r="R22" s="112"/>
       <c r="S22" s="32" t="s">
         <v>50</v>
       </c>
@@ -9325,7 +9343,7 @@
         <f>DEC2HEX('ipv4'!G23)</f>
         <v>16</v>
       </c>
-      <c r="H23" s="85"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="55"/>
       <c r="M23" s="48"/>
       <c r="P23" s="54" t="s">
@@ -9335,7 +9353,7 @@
         <f>DEC2HEX('ipv4'!Q29)</f>
         <v>E</v>
       </c>
-      <c r="R23" s="103"/>
+      <c r="R23" s="112"/>
       <c r="S23" s="64" t="s">
         <v>112</v>
       </c>
@@ -9360,13 +9378,13 @@
         <f>DEC2HEX('ipv4'!G24)</f>
         <v>17</v>
       </c>
-      <c r="H24" s="85"/>
+      <c r="H24" s="82"/>
       <c r="I24" s="55"/>
       <c r="K24" s="9" t="s">
         <v>96</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="114" t="s">
+      <c r="M24" s="102" t="s">
         <v>24</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -9376,7 +9394,7 @@
         <v>103</v>
       </c>
       <c r="Q24" s="33"/>
-      <c r="R24" s="103"/>
+      <c r="R24" s="112"/>
       <c r="S24" s="4" t="s">
         <v>23</v>
       </c>
@@ -9401,7 +9419,7 @@
         <f>DEC2HEX('ipv4'!G25)</f>
         <v>18</v>
       </c>
-      <c r="H25" s="85"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="55"/>
       <c r="K25" s="10" t="s">
         <v>96</v>
@@ -9410,16 +9428,16 @@
         <f>DEC2HEX('ipv4'!L33)</f>
         <v>1</v>
       </c>
-      <c r="M25" s="115"/>
+      <c r="M25" s="103"/>
       <c r="N25" s="55"/>
       <c r="P25" s="54" t="s">
         <v>103</v>
       </c>
       <c r="Q25" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q32)</f>
+        <f>DEC2HEX('ipv4'!Q33)</f>
         <v>1</v>
       </c>
-      <c r="R25" s="103"/>
+      <c r="R25" s="112"/>
       <c r="S25" s="32" t="s">
         <v>43</v>
       </c>
@@ -9441,7 +9459,7 @@
         <f>DEC2HEX('ipv4'!G26)</f>
         <v>19</v>
       </c>
-      <c r="H26" s="85"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="55"/>
       <c r="K26" s="10" t="s">
         <v>96</v>
@@ -9450,16 +9468,16 @@
         <f>DEC2HEX('ipv4'!L34)</f>
         <v>2</v>
       </c>
-      <c r="M26" s="115"/>
+      <c r="M26" s="103"/>
       <c r="N26" s="56"/>
       <c r="P26" s="54" t="s">
         <v>103</v>
       </c>
       <c r="Q26" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q33)</f>
+        <f>DEC2HEX('ipv4'!Q34)</f>
         <v>2</v>
       </c>
-      <c r="R26" s="103"/>
+      <c r="R26" s="112"/>
       <c r="S26" s="32" t="s">
         <v>52</v>
       </c>
@@ -9481,13 +9499,13 @@
         <f>DEC2HEX('ipv4'!G27)</f>
         <v>1A</v>
       </c>
-      <c r="H27" s="85"/>
+      <c r="H27" s="82"/>
       <c r="I27" s="55"/>
       <c r="K27" s="9" t="s">
         <v>97</v>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="115"/>
+      <c r="M27" s="103"/>
       <c r="N27" s="4" t="s">
         <v>23</v>
       </c>
@@ -9495,10 +9513,10 @@
         <v>103</v>
       </c>
       <c r="Q27" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q34)</f>
+        <f>DEC2HEX('ipv4'!Q35)</f>
         <v>3</v>
       </c>
-      <c r="R27" s="103"/>
+      <c r="R27" s="112"/>
       <c r="S27" s="32"/>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9518,7 +9536,7 @@
         <f>DEC2HEX('ipv4'!G28)</f>
         <v>1B</v>
       </c>
-      <c r="H28" s="85"/>
+      <c r="H28" s="82"/>
       <c r="I28" s="55"/>
       <c r="K28" s="10" t="s">
         <v>97</v>
@@ -9527,13 +9545,13 @@
         <f>DEC2HEX('ipv4'!L38)</f>
         <v>1</v>
       </c>
-      <c r="M28" s="115"/>
+      <c r="M28" s="103"/>
       <c r="N28" s="55"/>
       <c r="P28" s="53" t="s">
         <v>104</v>
       </c>
       <c r="Q28" s="33"/>
-      <c r="R28" s="103"/>
+      <c r="R28" s="112"/>
       <c r="S28" s="4" t="s">
         <v>23</v>
       </c>
@@ -9555,7 +9573,7 @@
         <f>DEC2HEX('ipv4'!G29)</f>
         <v>1C</v>
       </c>
-      <c r="H29" s="85"/>
+      <c r="H29" s="82"/>
       <c r="I29" s="55"/>
       <c r="K29" s="10" t="s">
         <v>97</v>
@@ -9564,16 +9582,16 @@
         <f>DEC2HEX('ipv4'!L39)</f>
         <v>2</v>
       </c>
-      <c r="M29" s="115"/>
+      <c r="M29" s="103"/>
       <c r="N29" s="55"/>
       <c r="P29" s="54" t="s">
         <v>104</v>
       </c>
       <c r="Q29" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q38)</f>
+        <f>DEC2HEX('ipv4'!Q39)</f>
         <v>1</v>
       </c>
-      <c r="R29" s="103"/>
+      <c r="R29" s="112"/>
       <c r="S29" s="32" t="s">
         <v>45</v>
       </c>
@@ -9595,13 +9613,13 @@
         <f>DEC2HEX('ipv4'!G30)</f>
         <v>1D</v>
       </c>
-      <c r="H30" s="85"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="55"/>
       <c r="K30" s="49" t="s">
         <v>98</v>
       </c>
       <c r="L30" s="50"/>
-      <c r="M30" s="115"/>
+      <c r="M30" s="103"/>
       <c r="N30" s="51" t="s">
         <v>23</v>
       </c>
@@ -9609,10 +9627,10 @@
         <v>104</v>
       </c>
       <c r="Q30" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q39)</f>
+        <f>DEC2HEX('ipv4'!Q40)</f>
         <v>2</v>
       </c>
-      <c r="R30" s="103"/>
+      <c r="R30" s="112"/>
       <c r="S30" s="32" t="s">
         <v>47</v>
       </c>
@@ -9634,7 +9652,7 @@
         <f>DEC2HEX('ipv4'!G31)</f>
         <v>1E</v>
       </c>
-      <c r="H31" s="85"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="55"/>
       <c r="K31" s="10" t="s">
         <v>98</v>
@@ -9643,16 +9661,16 @@
         <f>DEC2HEX('ipv4'!L43)</f>
         <v>1</v>
       </c>
-      <c r="M31" s="115"/>
+      <c r="M31" s="103"/>
       <c r="N31" s="55"/>
       <c r="P31" s="54" t="s">
         <v>104</v>
       </c>
       <c r="Q31" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q41)</f>
+        <f>DEC2HEX('ipv4'!Q42)</f>
         <v>4</v>
       </c>
-      <c r="R31" s="103"/>
+      <c r="R31" s="112"/>
       <c r="S31" s="70"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -9672,7 +9690,7 @@
         <f>DEC2HEX('ipv4'!G32)</f>
         <v>FE</v>
       </c>
-      <c r="H32" s="86"/>
+      <c r="H32" s="83"/>
       <c r="I32" s="7"/>
       <c r="K32" s="10" t="s">
         <v>98</v>
@@ -9681,16 +9699,16 @@
         <f>DEC2HEX('ipv4'!L44)</f>
         <v>2</v>
       </c>
-      <c r="M32" s="116"/>
+      <c r="M32" s="104"/>
       <c r="N32" s="55"/>
       <c r="P32" s="54" t="s">
         <v>104</v>
       </c>
       <c r="Q32" s="54" t="str">
-        <f>DEC2HEX('ipv4'!Q42)</f>
+        <f>DEC2HEX('ipv4'!Q43)</f>
         <v>5</v>
       </c>
-      <c r="R32" s="103"/>
+      <c r="R32" s="112"/>
       <c r="S32" s="32" t="s">
         <v>46</v>
       </c>
@@ -9713,10 +9731,10 @@
         <v>104</v>
       </c>
       <c r="Q33" s="54" t="str">
-        <f>DEC2HEX('ipv4'!Q43)</f>
-        <v>6</v>
-      </c>
-      <c r="R33" s="103"/>
+        <f>DEC2HEX('ipv4'!Q44)</f>
+        <v>6</v>
+      </c>
+      <c r="R33" s="112"/>
       <c r="S33" s="32" t="s">
         <v>48</v>
       </c>
@@ -9735,7 +9753,7 @@
         <v>84</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="99" t="s">
+      <c r="H34" s="108" t="s">
         <v>15</v>
       </c>
       <c r="I34" s="4" t="s">
@@ -9745,10 +9763,10 @@
         <v>104</v>
       </c>
       <c r="Q34" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q45)</f>
+        <f>DEC2HEX('ipv4'!Q46)</f>
         <v>8</v>
       </c>
-      <c r="R34" s="103"/>
+      <c r="R34" s="112"/>
       <c r="S34" s="70"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -9768,16 +9786,16 @@
         <f>DEC2HEX('ipv4'!G36)</f>
         <v>1</v>
       </c>
-      <c r="H35" s="100"/>
+      <c r="H35" s="109"/>
       <c r="I35" s="55"/>
       <c r="P35" s="54" t="s">
         <v>104</v>
       </c>
       <c r="Q35" s="54" t="str">
-        <f>DEC2HEX('ipv4'!Q46)</f>
+        <f>DEC2HEX('ipv4'!Q47)</f>
         <v>9</v>
       </c>
-      <c r="R35" s="103"/>
+      <c r="R35" s="112"/>
       <c r="S35" s="32" t="s">
         <v>55</v>
       </c>
@@ -9799,16 +9817,16 @@
         <f>DEC2HEX('ipv4'!G37)</f>
         <v>2</v>
       </c>
-      <c r="H36" s="100"/>
+      <c r="H36" s="109"/>
       <c r="I36" s="55"/>
       <c r="P36" s="54" t="s">
         <v>104</v>
       </c>
       <c r="Q36" s="54" t="str">
-        <f>DEC2HEX('ipv4'!Q47)</f>
+        <f>DEC2HEX('ipv4'!Q48)</f>
         <v>A</v>
       </c>
-      <c r="R36" s="103"/>
+      <c r="R36" s="112"/>
       <c r="S36" s="32" t="s">
         <v>54</v>
       </c>
@@ -9830,13 +9848,13 @@
         <f>DEC2HEX('ipv4'!G38)</f>
         <v>3</v>
       </c>
-      <c r="H37" s="100"/>
+      <c r="H37" s="109"/>
       <c r="I37" s="55"/>
       <c r="P37" s="53" t="s">
         <v>105</v>
       </c>
       <c r="Q37" s="33"/>
-      <c r="R37" s="103"/>
+      <c r="R37" s="112"/>
       <c r="S37" s="4" t="s">
         <v>23</v>
       </c>
@@ -9858,16 +9876,16 @@
         <f>DEC2HEX('ipv4'!G39)</f>
         <v>4</v>
       </c>
-      <c r="H38" s="100"/>
+      <c r="H38" s="109"/>
       <c r="I38" s="55"/>
       <c r="P38" s="54" t="s">
         <v>105</v>
       </c>
       <c r="Q38" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q50)</f>
+        <f>DEC2HEX('ipv4'!Q70)</f>
         <v>1</v>
       </c>
-      <c r="R38" s="103"/>
+      <c r="R38" s="112"/>
       <c r="S38" s="32" t="s">
         <v>44</v>
       </c>
@@ -9889,16 +9907,16 @@
         <f>DEC2HEX('ipv4'!G40)</f>
         <v>5</v>
       </c>
-      <c r="H39" s="100"/>
+      <c r="H39" s="109"/>
       <c r="I39" s="55"/>
       <c r="P39" s="54" t="s">
         <v>105</v>
       </c>
       <c r="Q39" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q51)</f>
+        <f>DEC2HEX('ipv4'!Q71)</f>
         <v>2</v>
       </c>
-      <c r="R39" s="103"/>
+      <c r="R39" s="112"/>
       <c r="S39" s="32" t="s">
         <v>53</v>
       </c>
@@ -9920,16 +9938,16 @@
         <f>DEC2HEX('ipv4'!G41)</f>
         <v>6</v>
       </c>
-      <c r="H40" s="100"/>
+      <c r="H40" s="109"/>
       <c r="I40" s="55"/>
       <c r="P40" s="54" t="s">
         <v>105</v>
       </c>
       <c r="Q40" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q52)</f>
+        <f>DEC2HEX('ipv4'!Q72)</f>
         <v>3</v>
       </c>
-      <c r="R40" s="104"/>
+      <c r="R40" s="113"/>
       <c r="S40" s="32"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -9949,7 +9967,7 @@
         <f>DEC2HEX('ipv4'!G42)</f>
         <v>7</v>
       </c>
-      <c r="H41" s="100"/>
+      <c r="H41" s="109"/>
       <c r="I41" s="55"/>
     </row>
     <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9969,13 +9987,13 @@
         <f>DEC2HEX('ipv4'!G43)</f>
         <v>8</v>
       </c>
-      <c r="H42" s="100"/>
+      <c r="H42" s="109"/>
       <c r="I42" s="55"/>
       <c r="P42" s="33" t="s">
         <v>122</v>
       </c>
       <c r="Q42" s="33"/>
-      <c r="R42" s="105" t="s">
+      <c r="R42" s="114" t="s">
         <v>118</v>
       </c>
       <c r="S42" s="4" t="s">
@@ -9999,16 +10017,16 @@
         <f>DEC2HEX('ipv4'!G44)</f>
         <v>9</v>
       </c>
-      <c r="H43" s="100"/>
+      <c r="H43" s="109"/>
       <c r="I43" s="55"/>
       <c r="P43" s="54" t="s">
         <v>122</v>
       </c>
       <c r="Q43" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q57)</f>
+        <f>DEC2HEX('ipv4'!Q77)</f>
         <v>1</v>
       </c>
-      <c r="R43" s="106"/>
+      <c r="R43" s="115"/>
       <c r="S43" s="32" t="s">
         <v>108</v>
       </c>
@@ -10030,16 +10048,16 @@
         <f>DEC2HEX('ipv4'!G45)</f>
         <v>A</v>
       </c>
-      <c r="H44" s="101"/>
+      <c r="H44" s="110"/>
       <c r="I44" s="55"/>
       <c r="P44" s="54" t="s">
         <v>122</v>
       </c>
       <c r="Q44" s="32" t="str">
-        <f>DEC2HEX('ipv4'!Q58)</f>
+        <f>DEC2HEX('ipv4'!Q78)</f>
         <v>2</v>
       </c>
-      <c r="R44" s="107"/>
+      <c r="R44" s="116"/>
       <c r="S44" s="32" t="s">
         <v>107</v>
       </c>
@@ -11146,12 +11164,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="M1:M15"/>
-    <mergeCell ref="M17:M22"/>
-    <mergeCell ref="M24:M32"/>
-    <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="C1:C144"/>
     <mergeCell ref="H34:H44"/>
     <mergeCell ref="H1:H32"/>
@@ -11159,6 +11171,12 @@
     <mergeCell ref="R7:R9"/>
     <mergeCell ref="R11:R40"/>
     <mergeCell ref="R42:R44"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="M1:M15"/>
+    <mergeCell ref="M17:M22"/>
+    <mergeCell ref="M24:M32"/>
+    <mergeCell ref="AA3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>